<commit_message>
student can see sections
</commit_message>
<xml_diff>
--- a/wwwroot/horario_ejemplo.xlsx
+++ b/wwwroot/horario_ejemplo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\Scheduler\wwwroot\Uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\Scheduler\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F8F893-6819-4618-827F-279644FA6322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963E6A0A-A5A6-4CBF-A2E1-804CB555CE57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{8AA74B92-4F8B-41D0-9DCA-80F5538843FD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <author>Usuario de Windows</author>
   </authors>
   <commentList>
-    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{F9706E5F-A4BE-463C-9E02-83A6110F2CEE}">
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{F9706E5F-A4BE-463C-9E02-83A6110F2CEE}">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ3" authorId="0" shapeId="0" xr:uid="{9AD9CD40-0FF1-4A72-B392-70D38302749A}">
+    <comment ref="BA3" authorId="0" shapeId="0" xr:uid="{9AD9CD40-0FF1-4A72-B392-70D38302749A}">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V14" authorId="0" shapeId="0" xr:uid="{E895903F-0372-4441-B4A1-5822DD6CA16F}">
+    <comment ref="W14" authorId="0" shapeId="0" xr:uid="{E895903F-0372-4441-B4A1-5822DD6CA16F}">
       <text>
         <r>
           <rPr>
@@ -108,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V17" authorId="0" shapeId="0" xr:uid="{3A6172C7-DA0A-44D5-B959-72C7318FBF31}">
+    <comment ref="W17" authorId="0" shapeId="0" xr:uid="{3A6172C7-DA0A-44D5-B959-72C7318FBF31}">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF17" authorId="0" shapeId="0" xr:uid="{3F3EF09E-55C8-4F20-8486-A2F779F41414}">
+    <comment ref="AG17" authorId="0" shapeId="0" xr:uid="{3F3EF09E-55C8-4F20-8486-A2F779F41414}">
       <text>
         <r>
           <rPr>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="69">
   <si>
     <t>Profesor</t>
   </si>
@@ -365,13 +365,16 @@
   </si>
   <si>
     <t>*** Electivo - MCD: Extrac. Y Gest. Datos masivos</t>
+  </si>
+  <si>
+    <t>Estudiantes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,6 +479,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -527,7 +538,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -831,11 +842,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1102,9 +1124,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1199,88 +1218,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -1647,177 +1594,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A51573-365A-43C8-B53A-90394AAA9A61}">
-  <dimension ref="A1:BP33"/>
+  <dimension ref="A1:BQ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" customWidth="1"/>
     <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="68" width="2.85546875" customWidth="1"/>
+    <col min="4" max="69" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:69" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="137" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="131"/>
-      <c r="K1" s="131"/>
-      <c r="L1" s="131"/>
-      <c r="M1" s="132"/>
-      <c r="N1" s="130" t="s">
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="131"/>
-      <c r="P1" s="131"/>
-      <c r="Q1" s="131"/>
-      <c r="R1" s="131"/>
-      <c r="S1" s="131"/>
-      <c r="T1" s="131"/>
-      <c r="U1" s="131"/>
-      <c r="V1" s="131"/>
-      <c r="W1" s="131"/>
-      <c r="X1" s="132"/>
-      <c r="Y1" s="130" t="s">
+      <c r="P1" s="130"/>
+      <c r="Q1" s="130"/>
+      <c r="R1" s="130"/>
+      <c r="S1" s="130"/>
+      <c r="T1" s="130"/>
+      <c r="U1" s="130"/>
+      <c r="V1" s="130"/>
+      <c r="W1" s="130"/>
+      <c r="X1" s="130"/>
+      <c r="Y1" s="131"/>
+      <c r="Z1" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="131"/>
-      <c r="AA1" s="131"/>
-      <c r="AB1" s="131"/>
-      <c r="AC1" s="131"/>
-      <c r="AD1" s="131"/>
-      <c r="AE1" s="131"/>
-      <c r="AF1" s="131"/>
-      <c r="AG1" s="131"/>
-      <c r="AH1" s="131"/>
-      <c r="AI1" s="132"/>
-      <c r="AJ1" s="130" t="s">
+      <c r="AA1" s="130"/>
+      <c r="AB1" s="130"/>
+      <c r="AC1" s="130"/>
+      <c r="AD1" s="130"/>
+      <c r="AE1" s="130"/>
+      <c r="AF1" s="130"/>
+      <c r="AG1" s="130"/>
+      <c r="AH1" s="130"/>
+      <c r="AI1" s="130"/>
+      <c r="AJ1" s="131"/>
+      <c r="AK1" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="AK1" s="131"/>
-      <c r="AL1" s="131"/>
-      <c r="AM1" s="133"/>
-      <c r="AN1" s="133"/>
-      <c r="AO1" s="131"/>
-      <c r="AP1" s="131"/>
-      <c r="AQ1" s="131"/>
-      <c r="AR1" s="131"/>
-      <c r="AS1" s="131"/>
-      <c r="AT1" s="132"/>
-      <c r="AU1" s="130" t="s">
+      <c r="AL1" s="130"/>
+      <c r="AM1" s="130"/>
+      <c r="AN1" s="132"/>
+      <c r="AO1" s="132"/>
+      <c r="AP1" s="130"/>
+      <c r="AQ1" s="130"/>
+      <c r="AR1" s="130"/>
+      <c r="AS1" s="130"/>
+      <c r="AT1" s="130"/>
+      <c r="AU1" s="131"/>
+      <c r="AV1" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="131"/>
-      <c r="AW1" s="131"/>
-      <c r="AX1" s="131"/>
-      <c r="AY1" s="131"/>
-      <c r="AZ1" s="131"/>
-      <c r="BA1" s="131"/>
-      <c r="BB1" s="131"/>
-      <c r="BC1" s="131"/>
-      <c r="BD1" s="131"/>
-      <c r="BE1" s="132"/>
-      <c r="BF1" s="134" t="s">
+      <c r="AW1" s="130"/>
+      <c r="AX1" s="130"/>
+      <c r="AY1" s="130"/>
+      <c r="AZ1" s="130"/>
+      <c r="BA1" s="130"/>
+      <c r="BB1" s="130"/>
+      <c r="BC1" s="130"/>
+      <c r="BD1" s="130"/>
+      <c r="BE1" s="130"/>
+      <c r="BF1" s="131"/>
+      <c r="BG1" s="133" t="s">
         <v>7</v>
       </c>
-      <c r="BG1" s="135"/>
-      <c r="BH1" s="135"/>
-      <c r="BI1" s="135"/>
-      <c r="BJ1" s="135"/>
-      <c r="BK1" s="135"/>
-      <c r="BL1" s="135"/>
-      <c r="BM1" s="135"/>
-      <c r="BN1" s="135"/>
-      <c r="BO1" s="135"/>
-      <c r="BP1" s="136"/>
+      <c r="BH1" s="134"/>
+      <c r="BI1" s="134"/>
+      <c r="BJ1" s="134"/>
+      <c r="BK1" s="134"/>
+      <c r="BL1" s="134"/>
+      <c r="BM1" s="134"/>
+      <c r="BN1" s="134"/>
+      <c r="BO1" s="134"/>
+      <c r="BP1" s="134"/>
+      <c r="BQ1" s="135"/>
     </row>
-    <row r="2" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
+      <c r="C2" s="137">
+        <v>30</v>
+      </c>
+      <c r="D2" s="68"/>
       <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
+      <c r="F2" s="7"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8">
-        <v>22</v>
-      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="8"/>
       <c r="Q2" s="8">
         <v>22</v>
       </c>
-      <c r="R2" s="8"/>
+      <c r="R2" s="8">
+        <v>22</v>
+      </c>
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
       <c r="V2" s="8"/>
       <c r="W2" s="8"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="8" t="s">
+      <c r="X2" s="8"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" s="8"/>
       <c r="AB2" s="8"/>
       <c r="AC2" s="8"/>
       <c r="AD2" s="8"/>
-      <c r="AE2" s="13"/>
+      <c r="AE2" s="8"/>
       <c r="AF2" s="13"/>
       <c r="AG2" s="13"/>
       <c r="AH2" s="13"/>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="8">
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="8">
         <v>22</v>
       </c>
-      <c r="AK2" s="8">
+      <c r="AL2" s="8">
         <v>24</v>
       </c>
-      <c r="AL2" s="15">
+      <c r="AM2" s="15">
         <v>24</v>
       </c>
-      <c r="AM2" s="16"/>
       <c r="AN2" s="16"/>
-      <c r="AO2" s="17" t="s">
-        <v>11</v>
-      </c>
+      <c r="AO2" s="16"/>
       <c r="AP2" s="17" t="s">
         <v>11</v>
       </c>
       <c r="AQ2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AR2" s="18"/>
+      <c r="AR2" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="AS2" s="18"/>
-      <c r="AT2" s="19"/>
-      <c r="AU2" s="20"/>
-      <c r="AV2" s="21"/>
-      <c r="AW2" s="18"/>
+      <c r="AT2" s="18"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="21"/>
       <c r="AX2" s="18"/>
       <c r="AY2" s="18"/>
       <c r="AZ2" s="18"/>
@@ -1825,9 +1777,9 @@
       <c r="BB2" s="18"/>
       <c r="BC2" s="18"/>
       <c r="BD2" s="18"/>
-      <c r="BE2" s="19"/>
-      <c r="BF2" s="22"/>
-      <c r="BG2" s="23"/>
+      <c r="BE2" s="18"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="22"/>
       <c r="BH2" s="23"/>
       <c r="BI2" s="23"/>
       <c r="BJ2" s="23"/>
@@ -1836,84 +1788,87 @@
       <c r="BM2" s="23"/>
       <c r="BN2" s="23"/>
       <c r="BO2" s="23"/>
-      <c r="BP2" s="24"/>
+      <c r="BP2" s="23"/>
+      <c r="BQ2" s="24"/>
     </row>
-    <row r="3" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
+      <c r="C3" s="137">
+        <v>24</v>
+      </c>
+      <c r="D3" s="68"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="10"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
-      <c r="R3" s="8">
-        <v>22</v>
-      </c>
+      <c r="R3" s="8"/>
       <c r="S3" s="8">
         <v>22</v>
       </c>
-      <c r="T3" s="8"/>
+      <c r="T3" s="8">
+        <v>22</v>
+      </c>
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="12"/>
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
       <c r="AC3" s="8"/>
       <c r="AD3" s="8"/>
-      <c r="AE3" s="13"/>
+      <c r="AE3" s="8"/>
       <c r="AF3" s="13"/>
       <c r="AG3" s="13"/>
       <c r="AH3" s="13"/>
-      <c r="AI3" s="14"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="8">
+      <c r="AI3" s="13"/>
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="10"/>
+      <c r="AL3" s="8">
         <v>22</v>
       </c>
-      <c r="AL3" s="25"/>
-      <c r="AM3" s="16"/>
+      <c r="AM3" s="25"/>
       <c r="AN3" s="16"/>
-      <c r="AO3" s="18"/>
+      <c r="AO3" s="16"/>
       <c r="AP3" s="18"/>
-      <c r="AQ3" s="17" t="s">
-        <v>13</v>
-      </c>
+      <c r="AQ3" s="18"/>
       <c r="AR3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="AS3" s="18"/>
-      <c r="AT3" s="19"/>
-      <c r="AU3" s="20"/>
-      <c r="AV3" s="21"/>
-      <c r="AW3" s="18"/>
+      <c r="AS3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT3" s="18"/>
+      <c r="AU3" s="19"/>
+      <c r="AV3" s="20"/>
+      <c r="AW3" s="21"/>
       <c r="AX3" s="18"/>
       <c r="AY3" s="18"/>
-      <c r="AZ3" s="26">
+      <c r="AZ3" s="18"/>
+      <c r="BA3" s="26">
         <v>22</v>
       </c>
-      <c r="BA3" s="18"/>
       <c r="BB3" s="18"/>
       <c r="BC3" s="18"/>
       <c r="BD3" s="18"/>
-      <c r="BE3" s="19"/>
-      <c r="BF3" s="27"/>
-      <c r="BG3" s="28"/>
+      <c r="BE3" s="18"/>
+      <c r="BF3" s="19"/>
+      <c r="BG3" s="27"/>
       <c r="BH3" s="28"/>
       <c r="BI3" s="28"/>
       <c r="BJ3" s="28"/>
@@ -1922,32 +1877,35 @@
       <c r="BM3" s="28"/>
       <c r="BN3" s="28"/>
       <c r="BO3" s="28"/>
-      <c r="BP3" s="29"/>
+      <c r="BP3" s="28"/>
+      <c r="BQ3" s="29"/>
     </row>
-    <row r="4" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
+      <c r="C4" s="137">
+        <v>30</v>
+      </c>
+      <c r="D4" s="68"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="8">
-        <v>13</v>
-      </c>
+      <c r="H4" s="8"/>
       <c r="I4" s="8">
         <v>13</v>
       </c>
-      <c r="J4" s="8"/>
+      <c r="J4" s="8">
+        <v>13</v>
+      </c>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="10"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
@@ -1956,46 +1914,46 @@
       <c r="U4" s="8"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="12"/>
       <c r="AA4" s="8"/>
       <c r="AB4" s="8"/>
       <c r="AC4" s="8"/>
       <c r="AD4" s="8"/>
-      <c r="AE4" s="13"/>
+      <c r="AE4" s="8"/>
       <c r="AF4" s="13"/>
       <c r="AG4" s="13"/>
       <c r="AH4" s="13"/>
-      <c r="AI4" s="14"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="8"/>
-      <c r="AL4" s="25"/>
-      <c r="AM4" s="16"/>
+      <c r="AI4" s="13"/>
+      <c r="AJ4" s="14"/>
+      <c r="AK4" s="10"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="25"/>
       <c r="AN4" s="16"/>
-      <c r="AO4" s="18"/>
+      <c r="AO4" s="16"/>
       <c r="AP4" s="18"/>
       <c r="AQ4" s="18"/>
       <c r="AR4" s="18"/>
       <c r="AS4" s="18"/>
-      <c r="AT4" s="19"/>
-      <c r="AU4" s="20"/>
-      <c r="AV4" s="21"/>
-      <c r="AW4" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="AT4" s="18"/>
+      <c r="AU4" s="19"/>
+      <c r="AV4" s="20"/>
+      <c r="AW4" s="21"/>
       <c r="AX4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="AY4" s="18"/>
+      <c r="AY4" s="17" t="s">
+        <v>16</v>
+      </c>
       <c r="AZ4" s="18"/>
       <c r="BA4" s="18"/>
       <c r="BB4" s="18"/>
       <c r="BC4" s="18"/>
       <c r="BD4" s="18"/>
-      <c r="BE4" s="19"/>
-      <c r="BF4" s="27"/>
-      <c r="BG4" s="28"/>
+      <c r="BE4" s="18"/>
+      <c r="BF4" s="19"/>
+      <c r="BG4" s="27"/>
       <c r="BH4" s="28"/>
       <c r="BI4" s="28"/>
       <c r="BJ4" s="28"/>
@@ -2004,32 +1962,35 @@
       <c r="BM4" s="28"/>
       <c r="BN4" s="28"/>
       <c r="BO4" s="28"/>
-      <c r="BP4" s="29"/>
+      <c r="BP4" s="28"/>
+      <c r="BQ4" s="29"/>
     </row>
-    <row r="5" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="137">
+        <v>30</v>
+      </c>
+      <c r="D5" s="68"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
+      <c r="F5" s="7"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="J5" s="8"/>
       <c r="K5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="8"/>
+      <c r="L5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="10"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
@@ -2038,46 +1999,46 @@
       <c r="U5" s="8"/>
       <c r="V5" s="8"/>
       <c r="W5" s="8"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="12"/>
       <c r="AA5" s="8"/>
       <c r="AB5" s="8"/>
       <c r="AC5" s="8"/>
       <c r="AD5" s="8"/>
-      <c r="AE5" s="13"/>
+      <c r="AE5" s="8"/>
       <c r="AF5" s="13"/>
       <c r="AG5" s="13"/>
       <c r="AH5" s="13"/>
-      <c r="AI5" s="14"/>
-      <c r="AJ5" s="30"/>
-      <c r="AK5" s="13"/>
-      <c r="AL5" s="25"/>
-      <c r="AM5" s="16"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="30"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="25"/>
       <c r="AN5" s="16"/>
-      <c r="AO5" s="18"/>
+      <c r="AO5" s="16"/>
       <c r="AP5" s="18"/>
       <c r="AQ5" s="18"/>
       <c r="AR5" s="18"/>
       <c r="AS5" s="18"/>
-      <c r="AT5" s="19"/>
-      <c r="AU5" s="20"/>
-      <c r="AV5" s="21"/>
-      <c r="AW5" s="17" t="s">
-        <v>11</v>
-      </c>
+      <c r="AT5" s="18"/>
+      <c r="AU5" s="19"/>
+      <c r="AV5" s="20"/>
+      <c r="AW5" s="21"/>
       <c r="AX5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AY5" s="18"/>
+      <c r="AY5" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="AZ5" s="18"/>
       <c r="BA5" s="18"/>
       <c r="BB5" s="18"/>
       <c r="BC5" s="18"/>
       <c r="BD5" s="18"/>
-      <c r="BE5" s="19"/>
-      <c r="BF5" s="27"/>
-      <c r="BG5" s="28"/>
+      <c r="BE5" s="18"/>
+      <c r="BF5" s="19"/>
+      <c r="BG5" s="27"/>
       <c r="BH5" s="28"/>
       <c r="BI5" s="28"/>
       <c r="BJ5" s="28"/>
@@ -2086,28 +2047,31 @@
       <c r="BM5" s="28"/>
       <c r="BN5" s="28"/>
       <c r="BO5" s="28"/>
-      <c r="BP5" s="29"/>
+      <c r="BP5" s="28"/>
+      <c r="BQ5" s="29"/>
     </row>
-    <row r="6" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="137">
+        <v>35</v>
+      </c>
+      <c r="D6" s="68"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="10"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
@@ -2116,40 +2080,40 @@
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
       <c r="W6" s="8"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="8"/>
       <c r="AB6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AC6" s="8"/>
+      <c r="AC6" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="AD6" s="8"/>
-      <c r="AE6" s="13"/>
+      <c r="AE6" s="8"/>
       <c r="AF6" s="13"/>
       <c r="AG6" s="13"/>
       <c r="AH6" s="13"/>
-      <c r="AI6" s="14"/>
-      <c r="AJ6" s="30"/>
-      <c r="AK6" s="13"/>
-      <c r="AL6" s="25"/>
-      <c r="AM6" s="16"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="14"/>
+      <c r="AK6" s="30"/>
+      <c r="AL6" s="13"/>
+      <c r="AM6" s="25"/>
       <c r="AN6" s="16"/>
-      <c r="AO6" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="AO6" s="16"/>
       <c r="AP6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="AQ6" s="18"/>
+      <c r="AQ6" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="AR6" s="18"/>
       <c r="AS6" s="18"/>
-      <c r="AT6" s="19"/>
-      <c r="AU6" s="20"/>
-      <c r="AV6" s="21"/>
-      <c r="AW6" s="18"/>
+      <c r="AT6" s="18"/>
+      <c r="AU6" s="19"/>
+      <c r="AV6" s="20"/>
+      <c r="AW6" s="21"/>
       <c r="AX6" s="18"/>
       <c r="AY6" s="18"/>
       <c r="AZ6" s="18"/>
@@ -2157,9 +2121,9 @@
       <c r="BB6" s="18"/>
       <c r="BC6" s="18"/>
       <c r="BD6" s="18"/>
-      <c r="BE6" s="19"/>
-      <c r="BF6" s="27"/>
-      <c r="BG6" s="28"/>
+      <c r="BE6" s="18"/>
+      <c r="BF6" s="19"/>
+      <c r="BG6" s="27"/>
       <c r="BH6" s="28"/>
       <c r="BI6" s="28"/>
       <c r="BJ6" s="28"/>
@@ -2168,28 +2132,31 @@
       <c r="BM6" s="28"/>
       <c r="BN6" s="28"/>
       <c r="BO6" s="28"/>
-      <c r="BP6" s="29"/>
+      <c r="BP6" s="28"/>
+      <c r="BQ6" s="29"/>
     </row>
-    <row r="7" spans="1:68" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:69" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
+      <c r="C7" s="137">
+        <v>35</v>
+      </c>
+      <c r="D7" s="68"/>
       <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="10"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
@@ -2198,40 +2165,40 @@
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="8"/>
       <c r="AB7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AC7" s="8"/>
+      <c r="AC7" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="AD7" s="8"/>
-      <c r="AE7" s="13"/>
+      <c r="AE7" s="8"/>
       <c r="AF7" s="13"/>
       <c r="AG7" s="13"/>
       <c r="AH7" s="13"/>
-      <c r="AI7" s="14"/>
-      <c r="AJ7" s="30"/>
-      <c r="AK7" s="13"/>
-      <c r="AL7" s="25"/>
-      <c r="AM7" s="16"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="14"/>
+      <c r="AK7" s="30"/>
+      <c r="AL7" s="13"/>
+      <c r="AM7" s="25"/>
       <c r="AN7" s="16"/>
-      <c r="AO7" s="18"/>
+      <c r="AO7" s="16"/>
       <c r="AP7" s="18"/>
-      <c r="AQ7" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="AQ7" s="18"/>
       <c r="AR7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="AS7" s="18"/>
-      <c r="AT7" s="19"/>
-      <c r="AU7" s="20"/>
-      <c r="AV7" s="21"/>
-      <c r="AW7" s="18"/>
+      <c r="AS7" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT7" s="18"/>
+      <c r="AU7" s="19"/>
+      <c r="AV7" s="20"/>
+      <c r="AW7" s="21"/>
       <c r="AX7" s="18"/>
       <c r="AY7" s="18"/>
       <c r="AZ7" s="18"/>
@@ -2239,9 +2206,9 @@
       <c r="BB7" s="18"/>
       <c r="BC7" s="18"/>
       <c r="BD7" s="18"/>
-      <c r="BE7" s="19"/>
-      <c r="BF7" s="27"/>
-      <c r="BG7" s="28"/>
+      <c r="BE7" s="18"/>
+      <c r="BF7" s="19"/>
+      <c r="BG7" s="27"/>
       <c r="BH7" s="28"/>
       <c r="BI7" s="28"/>
       <c r="BJ7" s="28"/>
@@ -2250,17 +2217,20 @@
       <c r="BM7" s="28"/>
       <c r="BN7" s="28"/>
       <c r="BO7" s="28"/>
-      <c r="BP7" s="29"/>
+      <c r="BP7" s="28"/>
+      <c r="BQ7" s="29"/>
     </row>
-    <row r="8" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
+      <c r="C8" s="137">
+        <v>47</v>
+      </c>
+      <c r="D8" s="39"/>
       <c r="E8" s="35"/>
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
@@ -2269,24 +2239,24 @@
       <c r="J8" s="35"/>
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="M8" s="35"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="37"/>
       <c r="P8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="Q8" s="8"/>
+      <c r="Q8" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
       <c r="U8" s="8"/>
-      <c r="V8" s="35"/>
+      <c r="V8" s="8"/>
       <c r="W8" s="35"/>
-      <c r="X8" s="38"/>
-      <c r="Y8" s="39"/>
-      <c r="Z8" s="35"/>
+      <c r="X8" s="35"/>
+      <c r="Y8" s="38"/>
+      <c r="Z8" s="39"/>
       <c r="AA8" s="35"/>
       <c r="AB8" s="35"/>
       <c r="AC8" s="35"/>
@@ -2295,33 +2265,33 @@
       <c r="AF8" s="35"/>
       <c r="AG8" s="35"/>
       <c r="AH8" s="35"/>
-      <c r="AI8" s="36"/>
-      <c r="AJ8" s="35"/>
+      <c r="AI8" s="35"/>
+      <c r="AJ8" s="36"/>
       <c r="AK8" s="35"/>
-      <c r="AL8" s="25"/>
-      <c r="AM8" s="16"/>
+      <c r="AL8" s="35"/>
+      <c r="AM8" s="25"/>
       <c r="AN8" s="16"/>
-      <c r="AO8" s="18"/>
+      <c r="AO8" s="16"/>
       <c r="AP8" s="18"/>
       <c r="AQ8" s="18"/>
       <c r="AR8" s="18"/>
       <c r="AS8" s="18"/>
-      <c r="AT8" s="19"/>
-      <c r="AU8" s="20"/>
-      <c r="AV8" s="21"/>
-      <c r="AW8" s="18"/>
+      <c r="AT8" s="18"/>
+      <c r="AU8" s="19"/>
+      <c r="AV8" s="20"/>
+      <c r="AW8" s="21"/>
       <c r="AX8" s="18"/>
       <c r="AY8" s="18"/>
-      <c r="AZ8" s="17" t="s">
+      <c r="AZ8" s="18"/>
+      <c r="BA8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="BA8" s="18"/>
       <c r="BB8" s="18"/>
       <c r="BC8" s="18"/>
       <c r="BD8" s="18"/>
-      <c r="BE8" s="19"/>
-      <c r="BF8" s="22"/>
-      <c r="BG8" s="23"/>
+      <c r="BE8" s="18"/>
+      <c r="BF8" s="19"/>
+      <c r="BG8" s="22"/>
       <c r="BH8" s="23"/>
       <c r="BI8" s="23"/>
       <c r="BJ8" s="23"/>
@@ -2330,17 +2300,20 @@
       <c r="BM8" s="23"/>
       <c r="BN8" s="23"/>
       <c r="BO8" s="23"/>
-      <c r="BP8" s="24"/>
+      <c r="BP8" s="23"/>
+      <c r="BQ8" s="24"/>
     </row>
-    <row r="9" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="40" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="35"/>
+      <c r="C9" s="137">
+        <v>32</v>
+      </c>
+      <c r="D9" s="39"/>
       <c r="E9" s="35"/>
       <c r="F9" s="35"/>
       <c r="G9" s="35"/>
@@ -2349,51 +2322,51 @@
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
       <c r="L9" s="35"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="8"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="37"/>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
-      <c r="T9" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="T9" s="8"/>
       <c r="U9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="V9" s="35"/>
+      <c r="V9" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="W9" s="35"/>
-      <c r="X9" s="38"/>
-      <c r="Y9" s="39"/>
-      <c r="Z9" s="35"/>
+      <c r="X9" s="35"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="39"/>
       <c r="AA9" s="35"/>
       <c r="AB9" s="35"/>
       <c r="AC9" s="35"/>
-      <c r="AD9" s="17" t="s">
-        <v>11</v>
-      </c>
+      <c r="AD9" s="35"/>
       <c r="AE9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AF9" s="35"/>
+      <c r="AF9" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="AG9" s="35"/>
       <c r="AH9" s="35"/>
-      <c r="AI9" s="36"/>
-      <c r="AJ9" s="34"/>
-      <c r="AK9" s="35"/>
-      <c r="AL9" s="25"/>
-      <c r="AM9" s="16"/>
+      <c r="AI9" s="35"/>
+      <c r="AJ9" s="36"/>
+      <c r="AK9" s="34"/>
+      <c r="AL9" s="35"/>
+      <c r="AM9" s="25"/>
       <c r="AN9" s="16"/>
-      <c r="AO9" s="18"/>
+      <c r="AO9" s="16"/>
       <c r="AP9" s="18"/>
       <c r="AQ9" s="18"/>
       <c r="AR9" s="18"/>
       <c r="AS9" s="18"/>
-      <c r="AT9" s="19"/>
-      <c r="AU9" s="20"/>
-      <c r="AV9" s="21"/>
-      <c r="AW9" s="18"/>
+      <c r="AT9" s="18"/>
+      <c r="AU9" s="19"/>
+      <c r="AV9" s="20"/>
+      <c r="AW9" s="21"/>
       <c r="AX9" s="18"/>
       <c r="AY9" s="18"/>
       <c r="AZ9" s="18"/>
@@ -2401,9 +2374,9 @@
       <c r="BB9" s="18"/>
       <c r="BC9" s="18"/>
       <c r="BD9" s="18"/>
-      <c r="BE9" s="19"/>
-      <c r="BF9" s="42"/>
-      <c r="BG9" s="43"/>
+      <c r="BE9" s="18"/>
+      <c r="BF9" s="19"/>
+      <c r="BG9" s="42"/>
       <c r="BH9" s="43"/>
       <c r="BI9" s="43"/>
       <c r="BJ9" s="43"/>
@@ -2412,17 +2385,20 @@
       <c r="BM9" s="43"/>
       <c r="BN9" s="43"/>
       <c r="BO9" s="43"/>
-      <c r="BP9" s="44"/>
+      <c r="BP9" s="43"/>
+      <c r="BQ9" s="44"/>
     </row>
-    <row r="10" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="45" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="137">
+        <v>15</v>
+      </c>
+      <c r="D10" s="68"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -2431,53 +2407,53 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="8">
-        <v>104</v>
-      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="48"/>
       <c r="R10" s="8">
         <v>104</v>
       </c>
-      <c r="S10" s="48"/>
+      <c r="S10" s="8">
+        <v>104</v>
+      </c>
       <c r="T10" s="48"/>
       <c r="U10" s="48"/>
       <c r="V10" s="48"/>
       <c r="W10" s="48"/>
-      <c r="X10" s="49"/>
-      <c r="Y10" s="50"/>
-      <c r="Z10" s="48"/>
+      <c r="X10" s="48"/>
+      <c r="Y10" s="49"/>
+      <c r="Z10" s="50"/>
       <c r="AA10" s="48"/>
       <c r="AB10" s="48"/>
       <c r="AC10" s="48"/>
       <c r="AD10" s="48"/>
-      <c r="AE10" s="48" t="s">
+      <c r="AE10" s="48"/>
+      <c r="AF10" s="48" t="s">
         <v>31</v>
-      </c>
-      <c r="AF10" s="51" t="s">
-        <v>11</v>
       </c>
       <c r="AG10" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="AH10" s="52"/>
-      <c r="AI10" s="53"/>
-      <c r="AJ10" s="54"/>
-      <c r="AK10" s="52"/>
-      <c r="AL10" s="25"/>
-      <c r="AM10" s="16"/>
+      <c r="AH10" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI10" s="52"/>
+      <c r="AJ10" s="53"/>
+      <c r="AK10" s="54"/>
+      <c r="AL10" s="52"/>
+      <c r="AM10" s="25"/>
       <c r="AN10" s="16"/>
-      <c r="AO10" s="55"/>
+      <c r="AO10" s="16"/>
       <c r="AP10" s="55"/>
       <c r="AQ10" s="55"/>
       <c r="AR10" s="55"/>
       <c r="AS10" s="55"/>
-      <c r="AT10" s="56"/>
-      <c r="AU10" s="57"/>
-      <c r="AV10" s="58"/>
-      <c r="AW10" s="55"/>
+      <c r="AT10" s="55"/>
+      <c r="AU10" s="56"/>
+      <c r="AV10" s="57"/>
+      <c r="AW10" s="58"/>
       <c r="AX10" s="55"/>
       <c r="AY10" s="55"/>
       <c r="AZ10" s="55"/>
@@ -2485,9 +2461,9 @@
       <c r="BB10" s="55"/>
       <c r="BC10" s="55"/>
       <c r="BD10" s="55"/>
-      <c r="BE10" s="56"/>
-      <c r="BF10" s="42"/>
-      <c r="BG10" s="43"/>
+      <c r="BE10" s="55"/>
+      <c r="BF10" s="56"/>
+      <c r="BG10" s="42"/>
       <c r="BH10" s="43"/>
       <c r="BI10" s="43"/>
       <c r="BJ10" s="43"/>
@@ -2496,17 +2472,20 @@
       <c r="BM10" s="43"/>
       <c r="BN10" s="43"/>
       <c r="BO10" s="43"/>
-      <c r="BP10" s="44"/>
+      <c r="BP10" s="43"/>
+      <c r="BQ10" s="44"/>
     </row>
-    <row r="11" spans="1:68" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:69" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="59" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="137">
+        <v>17</v>
+      </c>
+      <c r="D11" s="68"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -2515,10 +2494,10 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="48"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="7"/>
       <c r="Q11" s="48"/>
       <c r="R11" s="48"/>
       <c r="S11" s="48"/>
@@ -2526,50 +2505,50 @@
       <c r="U11" s="48"/>
       <c r="V11" s="48"/>
       <c r="W11" s="48"/>
-      <c r="X11" s="49"/>
-      <c r="Y11" s="50"/>
-      <c r="Z11" s="48"/>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="49"/>
+      <c r="Z11" s="50"/>
       <c r="AA11" s="48"/>
       <c r="AB11" s="48"/>
       <c r="AC11" s="48"/>
       <c r="AD11" s="48"/>
       <c r="AE11" s="48"/>
-      <c r="AF11" s="52"/>
+      <c r="AF11" s="48"/>
       <c r="AG11" s="52"/>
       <c r="AH11" s="52"/>
-      <c r="AI11" s="53"/>
-      <c r="AJ11" s="54">
+      <c r="AI11" s="52"/>
+      <c r="AJ11" s="53"/>
+      <c r="AK11" s="54">
         <v>13</v>
       </c>
-      <c r="AK11" s="60">
+      <c r="AL11" s="60">
         <v>13</v>
       </c>
-      <c r="AL11" s="25"/>
-      <c r="AM11" s="16"/>
+      <c r="AM11" s="25"/>
       <c r="AN11" s="16"/>
-      <c r="AO11" s="55"/>
+      <c r="AO11" s="16"/>
       <c r="AP11" s="55"/>
       <c r="AQ11" s="55"/>
       <c r="AR11" s="55"/>
       <c r="AS11" s="55"/>
-      <c r="AT11" s="56"/>
-      <c r="AU11" s="57"/>
-      <c r="AV11" s="58"/>
-      <c r="AW11" s="55"/>
+      <c r="AT11" s="55"/>
+      <c r="AU11" s="56"/>
+      <c r="AV11" s="57"/>
+      <c r="AW11" s="58"/>
       <c r="AX11" s="55"/>
       <c r="AY11" s="55"/>
       <c r="AZ11" s="55"/>
-      <c r="BA11" s="51" t="s">
+      <c r="BA11" s="55"/>
+      <c r="BB11" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="BB11" s="51" t="s">
+      <c r="BC11" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="BC11" s="55"/>
       <c r="BD11" s="55"/>
-      <c r="BE11" s="56"/>
-      <c r="BF11" s="61"/>
-      <c r="BG11" s="62"/>
+      <c r="BE11" s="55"/>
+      <c r="BF11" s="56"/>
+      <c r="BG11" s="61"/>
       <c r="BH11" s="62"/>
       <c r="BI11" s="62"/>
       <c r="BJ11" s="62"/>
@@ -2578,34 +2557,37 @@
       <c r="BM11" s="62"/>
       <c r="BN11" s="62"/>
       <c r="BO11" s="62"/>
-      <c r="BP11" s="63"/>
+      <c r="BP11" s="62"/>
+      <c r="BQ11" s="63"/>
     </row>
-    <row r="12" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="64" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="137">
+        <v>15</v>
+      </c>
+      <c r="D12" s="68"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="66" t="s">
-        <v>35</v>
-      </c>
+      <c r="G12" s="7"/>
       <c r="H12" s="66" t="s">
         <v>35</v>
       </c>
       <c r="I12" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="7"/>
+      <c r="J12" s="66" t="s">
+        <v>35</v>
+      </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="6"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
@@ -2614,9 +2596,9 @@
       <c r="U12" s="7"/>
       <c r="V12" s="7"/>
       <c r="W12" s="7"/>
-      <c r="X12" s="67"/>
-      <c r="Y12" s="68"/>
-      <c r="Z12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="67"/>
+      <c r="Z12" s="68"/>
       <c r="AA12" s="7"/>
       <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
@@ -2625,31 +2607,31 @@
       <c r="AF12" s="7"/>
       <c r="AG12" s="7"/>
       <c r="AH12" s="7"/>
-      <c r="AI12" s="47"/>
-      <c r="AJ12" s="6"/>
-      <c r="AK12" s="7"/>
-      <c r="AL12" s="69"/>
-      <c r="AM12" s="3"/>
+      <c r="AI12" s="7"/>
+      <c r="AJ12" s="47"/>
+      <c r="AK12" s="6"/>
+      <c r="AL12" s="7"/>
+      <c r="AM12" s="69"/>
       <c r="AN12" s="3"/>
-      <c r="AO12" s="70"/>
+      <c r="AO12" s="3"/>
       <c r="AP12" s="70"/>
       <c r="AQ12" s="70"/>
       <c r="AR12" s="70"/>
       <c r="AS12" s="70"/>
-      <c r="AT12" s="71"/>
-      <c r="AU12" s="72"/>
-      <c r="AV12" s="73"/>
-      <c r="AW12" s="70"/>
+      <c r="AT12" s="70"/>
+      <c r="AU12" s="71"/>
+      <c r="AV12" s="72"/>
+      <c r="AW12" s="73"/>
       <c r="AX12" s="70"/>
       <c r="AY12" s="70"/>
-      <c r="AZ12" s="18"/>
+      <c r="AZ12" s="70"/>
       <c r="BA12" s="18"/>
       <c r="BB12" s="18"/>
       <c r="BC12" s="18"/>
       <c r="BD12" s="18"/>
-      <c r="BE12" s="19"/>
-      <c r="BF12" s="74"/>
-      <c r="BG12" s="75"/>
+      <c r="BE12" s="18"/>
+      <c r="BF12" s="19"/>
+      <c r="BG12" s="74"/>
       <c r="BH12" s="75"/>
       <c r="BI12" s="75"/>
       <c r="BJ12" s="75"/>
@@ -2658,9 +2640,10 @@
       <c r="BM12" s="75"/>
       <c r="BN12" s="75"/>
       <c r="BO12" s="75"/>
-      <c r="BP12" s="76"/>
+      <c r="BP12" s="75"/>
+      <c r="BQ12" s="76"/>
     </row>
-    <row r="13" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
@@ -2668,14 +2651,13 @@
         <f>B12</f>
         <v>Proyecto de Programación - A</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
+      <c r="C13" s="137">
+        <v>15</v>
+      </c>
+      <c r="D13" s="68"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="66" t="str">
-        <f>G12</f>
-        <v>SP</v>
-      </c>
+      <c r="G13" s="7"/>
       <c r="H13" s="66" t="str">
         <f>H12</f>
         <v>SP</v>
@@ -2684,12 +2666,15 @@
         <f>I12</f>
         <v>SP</v>
       </c>
-      <c r="J13" s="7"/>
+      <c r="J13" s="66" t="str">
+        <f>J12</f>
+        <v>SP</v>
+      </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="6"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
@@ -2698,9 +2683,9 @@
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
-      <c r="X13" s="67"/>
-      <c r="Y13" s="68"/>
-      <c r="Z13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="67"/>
+      <c r="Z13" s="68"/>
       <c r="AA13" s="7"/>
       <c r="AB13" s="7"/>
       <c r="AC13" s="7"/>
@@ -2709,31 +2694,31 @@
       <c r="AF13" s="7"/>
       <c r="AG13" s="7"/>
       <c r="AH13" s="7"/>
-      <c r="AI13" s="47"/>
-      <c r="AJ13" s="6"/>
-      <c r="AK13" s="7"/>
-      <c r="AL13" s="69"/>
-      <c r="AM13" s="3"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="47"/>
+      <c r="AK13" s="6"/>
+      <c r="AL13" s="7"/>
+      <c r="AM13" s="69"/>
       <c r="AN13" s="3"/>
-      <c r="AO13" s="70"/>
+      <c r="AO13" s="3"/>
       <c r="AP13" s="70"/>
       <c r="AQ13" s="70"/>
       <c r="AR13" s="70"/>
       <c r="AS13" s="70"/>
-      <c r="AT13" s="71"/>
-      <c r="AU13" s="72"/>
-      <c r="AV13" s="73"/>
-      <c r="AW13" s="70"/>
+      <c r="AT13" s="70"/>
+      <c r="AU13" s="71"/>
+      <c r="AV13" s="72"/>
+      <c r="AW13" s="73"/>
       <c r="AX13" s="70"/>
       <c r="AY13" s="70"/>
-      <c r="AZ13" s="18"/>
+      <c r="AZ13" s="70"/>
       <c r="BA13" s="18"/>
       <c r="BB13" s="18"/>
       <c r="BC13" s="18"/>
       <c r="BD13" s="18"/>
-      <c r="BE13" s="19"/>
-      <c r="BF13" s="42"/>
-      <c r="BG13" s="43"/>
+      <c r="BE13" s="18"/>
+      <c r="BF13" s="19"/>
+      <c r="BG13" s="42"/>
       <c r="BH13" s="43"/>
       <c r="BI13" s="43"/>
       <c r="BJ13" s="43"/>
@@ -2742,45 +2727,48 @@
       <c r="BM13" s="43"/>
       <c r="BN13" s="43"/>
       <c r="BO13" s="43"/>
-      <c r="BP13" s="44"/>
+      <c r="BP13" s="43"/>
+      <c r="BQ13" s="44"/>
     </row>
-    <row r="14" spans="1:68" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:69" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="66" t="s">
-        <v>38</v>
-      </c>
+      <c r="C14" s="137">
+        <v>32</v>
+      </c>
+      <c r="D14" s="68"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="66" t="s">
+        <v>38</v>
+      </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="6"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
-      <c r="V14" s="7" t="s">
+      <c r="V14" s="7"/>
+      <c r="W14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="W14" s="7"/>
-      <c r="X14" s="67"/>
-      <c r="Y14" s="68"/>
-      <c r="Z14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="67"/>
+      <c r="Z14" s="68"/>
       <c r="AA14" s="7"/>
       <c r="AB14" s="7"/>
       <c r="AC14" s="7"/>
@@ -2789,35 +2777,35 @@
       <c r="AF14" s="7"/>
       <c r="AG14" s="7"/>
       <c r="AH14" s="7"/>
-      <c r="AI14" s="47"/>
-      <c r="AJ14" s="6"/>
-      <c r="AK14" s="7"/>
-      <c r="AL14" s="69"/>
-      <c r="AM14" s="3"/>
+      <c r="AI14" s="7"/>
+      <c r="AJ14" s="47"/>
+      <c r="AK14" s="6"/>
+      <c r="AL14" s="7"/>
+      <c r="AM14" s="69"/>
       <c r="AN14" s="3"/>
-      <c r="AO14" s="70"/>
+      <c r="AO14" s="3"/>
       <c r="AP14" s="70"/>
       <c r="AQ14" s="70"/>
       <c r="AR14" s="70"/>
       <c r="AS14" s="70"/>
-      <c r="AT14" s="71"/>
-      <c r="AU14" s="72"/>
-      <c r="AV14" s="73"/>
-      <c r="AW14" s="66" t="s">
-        <v>38</v>
-      </c>
+      <c r="AT14" s="70"/>
+      <c r="AU14" s="71"/>
+      <c r="AV14" s="72"/>
+      <c r="AW14" s="73"/>
       <c r="AX14" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="AY14" s="70"/>
-      <c r="AZ14" s="18"/>
+      <c r="AY14" s="66" t="s">
+        <v>38</v>
+      </c>
+      <c r="AZ14" s="70"/>
       <c r="BA14" s="18"/>
       <c r="BB14" s="18"/>
       <c r="BC14" s="18"/>
       <c r="BD14" s="18"/>
-      <c r="BE14" s="19"/>
-      <c r="BF14" s="42"/>
-      <c r="BG14" s="43"/>
+      <c r="BE14" s="18"/>
+      <c r="BF14" s="19"/>
+      <c r="BG14" s="42"/>
       <c r="BH14" s="43"/>
       <c r="BI14" s="43"/>
       <c r="BJ14" s="43"/>
@@ -2826,17 +2814,20 @@
       <c r="BM14" s="43"/>
       <c r="BN14" s="43"/>
       <c r="BO14" s="43"/>
-      <c r="BP14" s="44"/>
+      <c r="BP14" s="43"/>
+      <c r="BQ14" s="44"/>
     </row>
-    <row r="15" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="64" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="78"/>
+      <c r="C15" s="137">
+        <v>27</v>
+      </c>
+      <c r="D15" s="81"/>
       <c r="E15" s="78"/>
       <c r="F15" s="78"/>
       <c r="G15" s="78"/>
@@ -2845,9 +2836,9 @@
       <c r="J15" s="78"/>
       <c r="K15" s="78"/>
       <c r="L15" s="78"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="78"/>
+      <c r="M15" s="78"/>
+      <c r="N15" s="79"/>
+      <c r="O15" s="37"/>
       <c r="P15" s="78"/>
       <c r="Q15" s="78"/>
       <c r="R15" s="78"/>
@@ -2856,46 +2847,46 @@
       <c r="U15" s="78"/>
       <c r="V15" s="78"/>
       <c r="W15" s="78"/>
-      <c r="X15" s="80"/>
-      <c r="Y15" s="81"/>
-      <c r="Z15" s="48"/>
+      <c r="X15" s="78"/>
+      <c r="Y15" s="80"/>
+      <c r="Z15" s="81"/>
       <c r="AA15" s="48"/>
-      <c r="AB15" s="48" t="s">
-        <v>40</v>
-      </c>
+      <c r="AB15" s="48"/>
       <c r="AC15" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="AD15" s="48"/>
+      <c r="AD15" s="48" t="s">
+        <v>40</v>
+      </c>
       <c r="AE15" s="48"/>
       <c r="AF15" s="48"/>
       <c r="AG15" s="48"/>
       <c r="AH15" s="48"/>
-      <c r="AI15" s="79"/>
-      <c r="AJ15" s="37"/>
-      <c r="AK15" s="78"/>
-      <c r="AL15" s="82"/>
-      <c r="AM15" s="83"/>
+      <c r="AI15" s="48"/>
+      <c r="AJ15" s="79"/>
+      <c r="AK15" s="37"/>
+      <c r="AL15" s="78"/>
+      <c r="AM15" s="82"/>
       <c r="AN15" s="83"/>
-      <c r="AO15" s="84"/>
+      <c r="AO15" s="83"/>
       <c r="AP15" s="84"/>
       <c r="AQ15" s="84"/>
       <c r="AR15" s="84"/>
       <c r="AS15" s="84"/>
-      <c r="AT15" s="85"/>
-      <c r="AU15" s="86"/>
-      <c r="AV15" s="87"/>
-      <c r="AW15" s="84"/>
+      <c r="AT15" s="84"/>
+      <c r="AU15" s="85"/>
+      <c r="AV15" s="86"/>
+      <c r="AW15" s="87"/>
       <c r="AX15" s="84"/>
       <c r="AY15" s="84"/>
-      <c r="AZ15" s="18"/>
+      <c r="AZ15" s="84"/>
       <c r="BA15" s="18"/>
       <c r="BB15" s="18"/>
       <c r="BC15" s="18"/>
       <c r="BD15" s="18"/>
-      <c r="BE15" s="19"/>
-      <c r="BF15" s="74"/>
-      <c r="BG15" s="75"/>
+      <c r="BE15" s="18"/>
+      <c r="BF15" s="19"/>
+      <c r="BG15" s="74"/>
       <c r="BH15" s="75"/>
       <c r="BI15" s="75"/>
       <c r="BJ15" s="75"/>
@@ -2904,17 +2895,20 @@
       <c r="BM15" s="75"/>
       <c r="BN15" s="75"/>
       <c r="BO15" s="75"/>
-      <c r="BP15" s="76"/>
+      <c r="BP15" s="75"/>
+      <c r="BQ15" s="76"/>
     </row>
-    <row r="16" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="64" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="78"/>
+      <c r="C16" s="137">
+        <v>29</v>
+      </c>
+      <c r="D16" s="81"/>
       <c r="E16" s="78"/>
       <c r="F16" s="78"/>
       <c r="G16" s="78"/>
@@ -2923,9 +2917,9 @@
       <c r="J16" s="78"/>
       <c r="K16" s="78"/>
       <c r="L16" s="78"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="78"/>
+      <c r="M16" s="78"/>
+      <c r="N16" s="79"/>
+      <c r="O16" s="37"/>
       <c r="P16" s="78"/>
       <c r="Q16" s="78"/>
       <c r="R16" s="78"/>
@@ -2934,48 +2928,48 @@
       <c r="U16" s="78"/>
       <c r="V16" s="78"/>
       <c r="W16" s="78"/>
-      <c r="X16" s="80"/>
-      <c r="Y16" s="81"/>
-      <c r="Z16" s="48" t="s">
-        <v>35</v>
-      </c>
+      <c r="X16" s="78"/>
+      <c r="Y16" s="80"/>
+      <c r="Z16" s="81"/>
       <c r="AA16" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="AB16" s="48"/>
+      <c r="AB16" s="48" t="s">
+        <v>35</v>
+      </c>
       <c r="AC16" s="48"/>
       <c r="AD16" s="48"/>
       <c r="AE16" s="48"/>
       <c r="AF16" s="48"/>
       <c r="AG16" s="48"/>
       <c r="AH16" s="48"/>
-      <c r="AI16" s="79"/>
-      <c r="AJ16" s="37"/>
-      <c r="AK16" s="78"/>
-      <c r="AL16" s="82"/>
-      <c r="AM16" s="83"/>
+      <c r="AI16" s="48"/>
+      <c r="AJ16" s="79"/>
+      <c r="AK16" s="37"/>
+      <c r="AL16" s="78"/>
+      <c r="AM16" s="82"/>
       <c r="AN16" s="83"/>
-      <c r="AO16" s="84"/>
+      <c r="AO16" s="83"/>
       <c r="AP16" s="84"/>
       <c r="AQ16" s="84"/>
       <c r="AR16" s="84"/>
       <c r="AS16" s="84"/>
-      <c r="AT16" s="85"/>
-      <c r="AU16" s="86"/>
-      <c r="AV16" s="87"/>
-      <c r="AW16" s="84"/>
+      <c r="AT16" s="84"/>
+      <c r="AU16" s="85"/>
+      <c r="AV16" s="86"/>
+      <c r="AW16" s="87"/>
       <c r="AX16" s="84"/>
-      <c r="AY16" s="48">
+      <c r="AY16" s="84"/>
+      <c r="AZ16" s="48">
         <v>24</v>
       </c>
-      <c r="AZ16" s="18"/>
       <c r="BA16" s="18"/>
       <c r="BB16" s="18"/>
       <c r="BC16" s="18"/>
       <c r="BD16" s="18"/>
-      <c r="BE16" s="19"/>
-      <c r="BF16" s="42"/>
-      <c r="BG16" s="43"/>
+      <c r="BE16" s="18"/>
+      <c r="BF16" s="19"/>
+      <c r="BG16" s="42"/>
       <c r="BH16" s="43"/>
       <c r="BI16" s="43"/>
       <c r="BJ16" s="43"/>
@@ -2984,17 +2978,20 @@
       <c r="BM16" s="43"/>
       <c r="BN16" s="43"/>
       <c r="BO16" s="43"/>
-      <c r="BP16" s="44"/>
+      <c r="BP16" s="43"/>
+      <c r="BQ16" s="44"/>
     </row>
-    <row r="17" spans="1:68" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:69" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="64" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="78"/>
+      <c r="C17" s="137">
+        <v>13</v>
+      </c>
+      <c r="D17" s="81"/>
       <c r="E17" s="78"/>
       <c r="F17" s="78"/>
       <c r="G17" s="78"/>
@@ -3003,63 +3000,63 @@
       <c r="J17" s="78"/>
       <c r="K17" s="78"/>
       <c r="L17" s="78"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="78"/>
+      <c r="M17" s="78"/>
+      <c r="N17" s="79"/>
+      <c r="O17" s="37"/>
       <c r="P17" s="78"/>
       <c r="Q17" s="78"/>
-      <c r="R17" s="88" t="s">
+      <c r="R17" s="78"/>
+      <c r="S17" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="S17" s="78"/>
       <c r="T17" s="78"/>
       <c r="U17" s="78"/>
-      <c r="V17" s="78" t="s">
+      <c r="V17" s="78"/>
+      <c r="W17" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="W17" s="78"/>
-      <c r="X17" s="80"/>
-      <c r="Y17" s="81"/>
-      <c r="Z17" s="48"/>
+      <c r="X17" s="78"/>
+      <c r="Y17" s="80"/>
+      <c r="Z17" s="81"/>
       <c r="AA17" s="48"/>
       <c r="AB17" s="48"/>
       <c r="AC17" s="48"/>
-      <c r="AD17" s="48" t="s">
-        <v>38</v>
-      </c>
+      <c r="AD17" s="48"/>
       <c r="AE17" s="48" t="s">
         <v>38</v>
       </c>
       <c r="AF17" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG17" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="AG17" s="48"/>
       <c r="AH17" s="48"/>
-      <c r="AI17" s="79"/>
-      <c r="AJ17" s="37"/>
-      <c r="AK17" s="78"/>
-      <c r="AL17" s="82"/>
-      <c r="AM17" s="83"/>
+      <c r="AI17" s="48"/>
+      <c r="AJ17" s="79"/>
+      <c r="AK17" s="37"/>
+      <c r="AL17" s="78"/>
+      <c r="AM17" s="82"/>
       <c r="AN17" s="83"/>
-      <c r="AO17" s="84"/>
+      <c r="AO17" s="83"/>
       <c r="AP17" s="84"/>
       <c r="AQ17" s="84"/>
       <c r="AR17" s="84"/>
       <c r="AS17" s="84"/>
-      <c r="AT17" s="85"/>
-      <c r="AU17" s="86"/>
-      <c r="AV17" s="87"/>
-      <c r="AW17" s="84"/>
+      <c r="AT17" s="84"/>
+      <c r="AU17" s="85"/>
+      <c r="AV17" s="86"/>
+      <c r="AW17" s="87"/>
       <c r="AX17" s="84"/>
       <c r="AY17" s="84"/>
-      <c r="AZ17" s="18"/>
+      <c r="AZ17" s="84"/>
       <c r="BA17" s="18"/>
       <c r="BB17" s="18"/>
       <c r="BC17" s="18"/>
       <c r="BD17" s="18"/>
-      <c r="BE17" s="19"/>
-      <c r="BF17" s="42"/>
-      <c r="BG17" s="43"/>
+      <c r="BE17" s="18"/>
+      <c r="BF17" s="19"/>
+      <c r="BG17" s="42"/>
       <c r="BH17" s="43"/>
       <c r="BI17" s="43"/>
       <c r="BJ17" s="43"/>
@@ -3068,17 +3065,20 @@
       <c r="BM17" s="43"/>
       <c r="BN17" s="43"/>
       <c r="BO17" s="43"/>
-      <c r="BP17" s="44"/>
+      <c r="BP17" s="43"/>
+      <c r="BQ17" s="44"/>
     </row>
-    <row r="18" spans="1:68" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:69" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="64" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="35"/>
+      <c r="C18" s="137">
+        <v>24</v>
+      </c>
+      <c r="D18" s="39"/>
       <c r="E18" s="35"/>
       <c r="F18" s="35"/>
       <c r="G18" s="35"/>
@@ -3087,59 +3087,59 @@
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
       <c r="L18" s="35"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="34"/>
       <c r="P18" s="35"/>
       <c r="Q18" s="35"/>
       <c r="R18" s="35"/>
       <c r="S18" s="35"/>
       <c r="T18" s="35"/>
-      <c r="U18" s="17" t="s">
+      <c r="U18" s="35"/>
+      <c r="V18" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="V18" s="35"/>
       <c r="W18" s="35"/>
-      <c r="X18" s="38"/>
-      <c r="Y18" s="39"/>
-      <c r="Z18" s="35"/>
+      <c r="X18" s="35"/>
+      <c r="Y18" s="38"/>
+      <c r="Z18" s="39"/>
       <c r="AA18" s="35"/>
-      <c r="AB18" s="48">
-        <v>104</v>
-      </c>
+      <c r="AB18" s="35"/>
       <c r="AC18" s="48">
         <v>104</v>
       </c>
-      <c r="AD18" s="89"/>
-      <c r="AE18" s="35"/>
+      <c r="AD18" s="48">
+        <v>104</v>
+      </c>
+      <c r="AE18" s="89"/>
       <c r="AF18" s="35"/>
       <c r="AG18" s="35"/>
       <c r="AH18" s="35"/>
-      <c r="AI18" s="36"/>
-      <c r="AJ18" s="90"/>
-      <c r="AK18" s="91"/>
+      <c r="AI18" s="35"/>
+      <c r="AJ18" s="36"/>
+      <c r="AK18" s="90"/>
       <c r="AL18" s="91"/>
-      <c r="AM18" s="92"/>
-      <c r="AN18" s="16"/>
-      <c r="AO18" s="91"/>
+      <c r="AM18" s="91"/>
+      <c r="AN18" s="92"/>
+      <c r="AO18" s="16"/>
       <c r="AP18" s="91"/>
       <c r="AQ18" s="91"/>
       <c r="AR18" s="91"/>
       <c r="AS18" s="91"/>
-      <c r="AT18" s="93"/>
-      <c r="AU18" s="94"/>
-      <c r="AV18" s="95"/>
-      <c r="AW18" s="96"/>
+      <c r="AT18" s="91"/>
+      <c r="AU18" s="93"/>
+      <c r="AV18" s="94"/>
+      <c r="AW18" s="95"/>
       <c r="AX18" s="96"/>
-      <c r="AY18" s="95"/>
-      <c r="AZ18" s="96"/>
-      <c r="BA18" s="95"/>
+      <c r="AY18" s="96"/>
+      <c r="AZ18" s="95"/>
+      <c r="BA18" s="96"/>
       <c r="BB18" s="95"/>
       <c r="BC18" s="95"/>
-      <c r="BD18" s="96"/>
-      <c r="BE18" s="97"/>
-      <c r="BF18" s="74"/>
-      <c r="BG18" s="75"/>
+      <c r="BD18" s="95"/>
+      <c r="BE18" s="96"/>
+      <c r="BF18" s="97"/>
+      <c r="BG18" s="74"/>
       <c r="BH18" s="75"/>
       <c r="BI18" s="75"/>
       <c r="BJ18" s="75"/>
@@ -3148,47 +3148,50 @@
       <c r="BM18" s="75"/>
       <c r="BN18" s="75"/>
       <c r="BO18" s="75"/>
-      <c r="BP18" s="76"/>
+      <c r="BP18" s="75"/>
+      <c r="BQ18" s="76"/>
     </row>
-    <row r="19" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="64" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="98"/>
-      <c r="D19" s="48" t="s">
-        <v>18</v>
-      </c>
+      <c r="C19" s="137">
+        <v>20</v>
+      </c>
+      <c r="D19" s="50"/>
       <c r="E19" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="48"/>
+      <c r="F19" s="48" t="s">
+        <v>18</v>
+      </c>
       <c r="G19" s="48"/>
       <c r="H19" s="48"/>
       <c r="I19" s="48"/>
       <c r="J19" s="48"/>
       <c r="K19" s="48"/>
       <c r="L19" s="48"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="78"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="79"/>
+      <c r="O19" s="37"/>
       <c r="P19" s="78"/>
-      <c r="Q19" s="88" t="s">
-        <v>11</v>
-      </c>
+      <c r="Q19" s="78"/>
       <c r="R19" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="S19" s="78"/>
+      <c r="S19" s="88" t="s">
+        <v>11</v>
+      </c>
       <c r="T19" s="78"/>
       <c r="U19" s="78"/>
       <c r="V19" s="78"/>
       <c r="W19" s="78"/>
-      <c r="X19" s="80"/>
-      <c r="Y19" s="81"/>
-      <c r="Z19" s="78"/>
+      <c r="X19" s="78"/>
+      <c r="Y19" s="80"/>
+      <c r="Z19" s="81"/>
       <c r="AA19" s="78"/>
       <c r="AB19" s="78"/>
       <c r="AC19" s="78"/>
@@ -3197,31 +3200,31 @@
       <c r="AF19" s="78"/>
       <c r="AG19" s="78"/>
       <c r="AH19" s="78"/>
-      <c r="AI19" s="79"/>
-      <c r="AJ19" s="37"/>
-      <c r="AK19" s="78"/>
-      <c r="AL19" s="82"/>
-      <c r="AM19" s="83"/>
+      <c r="AI19" s="78"/>
+      <c r="AJ19" s="79"/>
+      <c r="AK19" s="37"/>
+      <c r="AL19" s="78"/>
+      <c r="AM19" s="82"/>
       <c r="AN19" s="83"/>
-      <c r="AO19" s="84"/>
+      <c r="AO19" s="83"/>
       <c r="AP19" s="84"/>
       <c r="AQ19" s="84"/>
       <c r="AR19" s="84"/>
       <c r="AS19" s="84"/>
-      <c r="AT19" s="85"/>
-      <c r="AU19" s="86"/>
-      <c r="AV19" s="87"/>
-      <c r="AW19" s="84"/>
+      <c r="AT19" s="84"/>
+      <c r="AU19" s="85"/>
+      <c r="AV19" s="86"/>
+      <c r="AW19" s="87"/>
       <c r="AX19" s="84"/>
       <c r="AY19" s="84"/>
       <c r="AZ19" s="84"/>
       <c r="BA19" s="84"/>
-      <c r="BB19" s="18"/>
+      <c r="BB19" s="84"/>
       <c r="BC19" s="18"/>
       <c r="BD19" s="18"/>
-      <c r="BE19" s="19"/>
-      <c r="BF19" s="74"/>
-      <c r="BG19" s="75"/>
+      <c r="BE19" s="18"/>
+      <c r="BF19" s="19"/>
+      <c r="BG19" s="74"/>
       <c r="BH19" s="75"/>
       <c r="BI19" s="75"/>
       <c r="BJ19" s="75"/>
@@ -3230,32 +3233,35 @@
       <c r="BM19" s="75"/>
       <c r="BN19" s="75"/>
       <c r="BO19" s="75"/>
-      <c r="BP19" s="76"/>
+      <c r="BP19" s="75"/>
+      <c r="BQ19" s="76"/>
     </row>
-    <row r="20" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="99" t="s">
+    <row r="20" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="99" t="s">
+      <c r="B20" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="98"/>
-      <c r="D20" s="48"/>
+      <c r="C20" s="137">
+        <v>16</v>
+      </c>
+      <c r="D20" s="50"/>
       <c r="E20" s="48"/>
-      <c r="F20" s="48" t="s">
-        <v>40</v>
-      </c>
+      <c r="F20" s="48"/>
       <c r="G20" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="H20" s="48"/>
+      <c r="H20" s="48" t="s">
+        <v>40</v>
+      </c>
       <c r="I20" s="48"/>
       <c r="J20" s="48"/>
       <c r="K20" s="48"/>
       <c r="L20" s="48"/>
-      <c r="M20" s="79"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="78"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="79"/>
+      <c r="O20" s="37"/>
       <c r="P20" s="78"/>
       <c r="Q20" s="78"/>
       <c r="R20" s="78"/>
@@ -3264,65 +3270,68 @@
       <c r="U20" s="78"/>
       <c r="V20" s="78"/>
       <c r="W20" s="78"/>
-      <c r="X20" s="80"/>
-      <c r="Y20" s="81"/>
-      <c r="Z20" s="78"/>
+      <c r="X20" s="78"/>
+      <c r="Y20" s="80"/>
+      <c r="Z20" s="81"/>
       <c r="AA20" s="78"/>
       <c r="AB20" s="78"/>
       <c r="AC20" s="78"/>
-      <c r="AD20" s="84"/>
+      <c r="AD20" s="78"/>
       <c r="AE20" s="84"/>
-      <c r="AF20" s="78"/>
+      <c r="AF20" s="84"/>
       <c r="AG20" s="78"/>
       <c r="AH20" s="78"/>
-      <c r="AI20" s="79"/>
-      <c r="AJ20" s="37"/>
-      <c r="AK20" s="78"/>
-      <c r="AL20" s="82"/>
-      <c r="AM20" s="83"/>
+      <c r="AI20" s="78"/>
+      <c r="AJ20" s="79"/>
+      <c r="AK20" s="37"/>
+      <c r="AL20" s="78"/>
+      <c r="AM20" s="82"/>
       <c r="AN20" s="83"/>
-      <c r="AO20" s="84"/>
+      <c r="AO20" s="83"/>
       <c r="AP20" s="84"/>
       <c r="AQ20" s="84"/>
       <c r="AR20" s="84"/>
       <c r="AS20" s="84"/>
-      <c r="AT20" s="85"/>
-      <c r="AU20" s="8">
+      <c r="AT20" s="84"/>
+      <c r="AU20" s="85"/>
+      <c r="AV20" s="8">
         <v>104</v>
       </c>
-      <c r="AV20" s="88" t="s">
+      <c r="AW20" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="AW20" s="84"/>
       <c r="AX20" s="84"/>
       <c r="AY20" s="84"/>
       <c r="AZ20" s="84"/>
       <c r="BA20" s="84"/>
-      <c r="BB20" s="18"/>
+      <c r="BB20" s="84"/>
       <c r="BC20" s="18"/>
       <c r="BD20" s="18"/>
-      <c r="BE20" s="19"/>
-      <c r="BF20" s="100"/>
-      <c r="BG20" s="101"/>
-      <c r="BH20" s="101"/>
-      <c r="BI20" s="101"/>
-      <c r="BJ20" s="101"/>
-      <c r="BK20" s="101"/>
-      <c r="BL20" s="101"/>
-      <c r="BM20" s="101"/>
-      <c r="BN20" s="101"/>
-      <c r="BO20" s="101"/>
-      <c r="BP20" s="102"/>
+      <c r="BE20" s="18"/>
+      <c r="BF20" s="19"/>
+      <c r="BG20" s="99"/>
+      <c r="BH20" s="100"/>
+      <c r="BI20" s="100"/>
+      <c r="BJ20" s="100"/>
+      <c r="BK20" s="100"/>
+      <c r="BL20" s="100"/>
+      <c r="BM20" s="100"/>
+      <c r="BN20" s="100"/>
+      <c r="BO20" s="100"/>
+      <c r="BP20" s="100"/>
+      <c r="BQ20" s="101"/>
     </row>
-    <row r="21" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="103" t="s">
+    <row r="21" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="102" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="98"/>
-      <c r="D21" s="48"/>
+      <c r="C21" s="137">
+        <v>8</v>
+      </c>
+      <c r="D21" s="50"/>
       <c r="E21" s="48"/>
       <c r="F21" s="48"/>
       <c r="G21" s="48"/>
@@ -3331,9 +3340,9 @@
       <c r="J21" s="48"/>
       <c r="K21" s="48"/>
       <c r="L21" s="48"/>
-      <c r="M21" s="79"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="78"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="79"/>
+      <c r="O21" s="37"/>
       <c r="P21" s="78"/>
       <c r="Q21" s="78"/>
       <c r="R21" s="78"/>
@@ -3342,82 +3351,85 @@
       <c r="U21" s="78"/>
       <c r="V21" s="78"/>
       <c r="W21" s="78"/>
-      <c r="X21" s="80"/>
-      <c r="Y21" s="81"/>
-      <c r="Z21" s="78"/>
-      <c r="AA21" s="88" t="s">
+      <c r="X21" s="78"/>
+      <c r="Y21" s="80"/>
+      <c r="Z21" s="81"/>
+      <c r="AA21" s="78"/>
+      <c r="AB21" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="AB21" s="78"/>
       <c r="AC21" s="78"/>
       <c r="AD21" s="78"/>
       <c r="AE21" s="78"/>
       <c r="AF21" s="78"/>
       <c r="AG21" s="78"/>
       <c r="AH21" s="78"/>
-      <c r="AI21" s="79"/>
-      <c r="AJ21" s="37"/>
-      <c r="AK21" s="78"/>
-      <c r="AL21" s="82"/>
-      <c r="AM21" s="83"/>
+      <c r="AI21" s="78"/>
+      <c r="AJ21" s="79"/>
+      <c r="AK21" s="37"/>
+      <c r="AL21" s="78"/>
+      <c r="AM21" s="82"/>
       <c r="AN21" s="83"/>
-      <c r="AO21" s="84"/>
+      <c r="AO21" s="83"/>
       <c r="AP21" s="84"/>
       <c r="AQ21" s="84"/>
       <c r="AR21" s="84"/>
       <c r="AS21" s="84"/>
-      <c r="AT21" s="85"/>
-      <c r="AU21" s="86"/>
-      <c r="AV21" s="87"/>
-      <c r="AW21" s="84"/>
+      <c r="AT21" s="84"/>
+      <c r="AU21" s="85"/>
+      <c r="AV21" s="86"/>
+      <c r="AW21" s="87"/>
       <c r="AX21" s="84"/>
-      <c r="AY21" s="12" t="s">
-        <v>31</v>
-      </c>
+      <c r="AY21" s="84"/>
       <c r="AZ21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="BA21" s="48"/>
-      <c r="BB21" s="18"/>
+      <c r="BA21" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB21" s="48"/>
       <c r="BC21" s="18"/>
       <c r="BD21" s="18"/>
-      <c r="BE21" s="19"/>
-      <c r="BF21" s="100"/>
-      <c r="BG21" s="101"/>
-      <c r="BH21" s="101"/>
-      <c r="BI21" s="101"/>
-      <c r="BJ21" s="101"/>
-      <c r="BK21" s="101"/>
-      <c r="BL21" s="101"/>
-      <c r="BM21" s="101"/>
-      <c r="BN21" s="101"/>
-      <c r="BO21" s="101"/>
-      <c r="BP21" s="102"/>
+      <c r="BE21" s="18"/>
+      <c r="BF21" s="19"/>
+      <c r="BG21" s="99"/>
+      <c r="BH21" s="100"/>
+      <c r="BI21" s="100"/>
+      <c r="BJ21" s="100"/>
+      <c r="BK21" s="100"/>
+      <c r="BL21" s="100"/>
+      <c r="BM21" s="100"/>
+      <c r="BN21" s="100"/>
+      <c r="BO21" s="100"/>
+      <c r="BP21" s="100"/>
+      <c r="BQ21" s="101"/>
     </row>
-    <row r="22" spans="1:68" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="99" t="s">
+    <row r="22" spans="1:69" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="99" t="s">
+      <c r="B22" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="78"/>
+      <c r="C22" s="137">
+        <v>9</v>
+      </c>
+      <c r="D22" s="81"/>
       <c r="E22" s="78"/>
       <c r="F22" s="78"/>
       <c r="G22" s="78"/>
-      <c r="H22" s="78" t="s">
-        <v>53</v>
-      </c>
+      <c r="H22" s="78"/>
       <c r="I22" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="J22" s="78"/>
+      <c r="J22" s="78" t="s">
+        <v>53</v>
+      </c>
       <c r="K22" s="78"/>
       <c r="L22" s="78"/>
-      <c r="M22" s="79"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="78"/>
+      <c r="M22" s="78"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="37"/>
       <c r="P22" s="78"/>
       <c r="Q22" s="78"/>
       <c r="R22" s="78"/>
@@ -3426,10 +3438,10 @@
       <c r="U22" s="78"/>
       <c r="V22" s="78"/>
       <c r="W22" s="78"/>
-      <c r="X22" s="80"/>
-      <c r="Y22" s="8"/>
+      <c r="X22" s="78"/>
+      <c r="Y22" s="80"/>
       <c r="Z22" s="8"/>
-      <c r="AA22" s="78"/>
+      <c r="AA22" s="8"/>
       <c r="AB22" s="78"/>
       <c r="AC22" s="78"/>
       <c r="AD22" s="78"/>
@@ -3437,54 +3449,57 @@
       <c r="AF22" s="78"/>
       <c r="AG22" s="78"/>
       <c r="AH22" s="78"/>
-      <c r="AI22" s="79"/>
-      <c r="AJ22" s="37"/>
-      <c r="AK22" s="78"/>
-      <c r="AL22" s="82"/>
-      <c r="AM22" s="83"/>
+      <c r="AI22" s="78"/>
+      <c r="AJ22" s="79"/>
+      <c r="AK22" s="37"/>
+      <c r="AL22" s="78"/>
+      <c r="AM22" s="82"/>
       <c r="AN22" s="83"/>
-      <c r="AO22" s="84"/>
+      <c r="AO22" s="83"/>
       <c r="AP22" s="84"/>
       <c r="AQ22" s="84"/>
       <c r="AR22" s="84"/>
       <c r="AS22" s="84"/>
-      <c r="AT22" s="85"/>
-      <c r="AU22" s="86"/>
-      <c r="AV22" s="87"/>
-      <c r="AW22" s="48">
-        <v>23</v>
-      </c>
+      <c r="AT22" s="84"/>
+      <c r="AU22" s="85"/>
+      <c r="AV22" s="86"/>
+      <c r="AW22" s="87"/>
       <c r="AX22" s="48">
         <v>23</v>
       </c>
-      <c r="AY22" s="84"/>
+      <c r="AY22" s="48">
+        <v>23</v>
+      </c>
       <c r="AZ22" s="84"/>
       <c r="BA22" s="84"/>
-      <c r="BB22" s="18"/>
+      <c r="BB22" s="84"/>
       <c r="BC22" s="18"/>
       <c r="BD22" s="18"/>
-      <c r="BE22" s="19"/>
-      <c r="BF22" s="100"/>
-      <c r="BG22" s="101"/>
-      <c r="BH22" s="101"/>
-      <c r="BI22" s="101"/>
-      <c r="BJ22" s="101"/>
-      <c r="BK22" s="101"/>
-      <c r="BL22" s="101"/>
-      <c r="BM22" s="101"/>
-      <c r="BN22" s="101"/>
-      <c r="BO22" s="101"/>
-      <c r="BP22" s="102"/>
+      <c r="BE22" s="18"/>
+      <c r="BF22" s="19"/>
+      <c r="BG22" s="99"/>
+      <c r="BH22" s="100"/>
+      <c r="BI22" s="100"/>
+      <c r="BJ22" s="100"/>
+      <c r="BK22" s="100"/>
+      <c r="BL22" s="100"/>
+      <c r="BM22" s="100"/>
+      <c r="BN22" s="100"/>
+      <c r="BO22" s="100"/>
+      <c r="BP22" s="100"/>
+      <c r="BQ22" s="101"/>
     </row>
-    <row r="23" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="104" t="s">
+      <c r="B23" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="78"/>
+      <c r="C23" s="137">
+        <v>21</v>
+      </c>
+      <c r="D23" s="81"/>
       <c r="E23" s="78"/>
       <c r="F23" s="78"/>
       <c r="G23" s="78"/>
@@ -3493,9 +3508,9 @@
       <c r="J23" s="78"/>
       <c r="K23" s="78"/>
       <c r="L23" s="78"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="78"/>
+      <c r="M23" s="78"/>
+      <c r="N23" s="79"/>
+      <c r="O23" s="37"/>
       <c r="P23" s="78"/>
       <c r="Q23" s="78"/>
       <c r="R23" s="78"/>
@@ -3504,9 +3519,9 @@
       <c r="U23" s="78"/>
       <c r="V23" s="78"/>
       <c r="W23" s="78"/>
-      <c r="X23" s="80"/>
-      <c r="Y23" s="81"/>
-      <c r="Z23" s="78"/>
+      <c r="X23" s="78"/>
+      <c r="Y23" s="80"/>
+      <c r="Z23" s="81"/>
       <c r="AA23" s="78"/>
       <c r="AB23" s="78"/>
       <c r="AC23" s="78"/>
@@ -3515,56 +3530,59 @@
       <c r="AF23" s="78"/>
       <c r="AG23" s="78"/>
       <c r="AH23" s="78"/>
-      <c r="AI23" s="79"/>
-      <c r="AJ23" s="37"/>
-      <c r="AK23" s="78"/>
-      <c r="AL23" s="82"/>
-      <c r="AM23" s="83"/>
+      <c r="AI23" s="78"/>
+      <c r="AJ23" s="79"/>
+      <c r="AK23" s="37"/>
+      <c r="AL23" s="78"/>
+      <c r="AM23" s="82"/>
       <c r="AN23" s="83"/>
-      <c r="AO23" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="AO23" s="83"/>
       <c r="AP23" s="8" t="s">
         <v>10</v>
       </c>
       <c r="AQ23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AR23" s="48"/>
-      <c r="AS23" s="84"/>
-      <c r="AT23" s="93"/>
-      <c r="AU23" s="90"/>
-      <c r="AV23" s="91"/>
+      <c r="AR23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AS23" s="48"/>
+      <c r="AT23" s="84"/>
+      <c r="AU23" s="93"/>
+      <c r="AV23" s="90"/>
       <c r="AW23" s="91"/>
-      <c r="AX23" s="105"/>
-      <c r="AY23" s="105"/>
-      <c r="AZ23" s="91"/>
+      <c r="AX23" s="91"/>
+      <c r="AY23" s="104"/>
+      <c r="AZ23" s="104"/>
       <c r="BA23" s="91"/>
       <c r="BB23" s="91"/>
       <c r="BC23" s="91"/>
       <c r="BD23" s="91"/>
-      <c r="BE23" s="93"/>
-      <c r="BF23" s="74"/>
-      <c r="BG23" s="95"/>
+      <c r="BE23" s="91"/>
+      <c r="BF23" s="93"/>
+      <c r="BG23" s="74"/>
       <c r="BH23" s="95"/>
-      <c r="BI23" s="106"/>
-      <c r="BJ23" s="75"/>
+      <c r="BI23" s="95"/>
+      <c r="BJ23" s="105"/>
       <c r="BK23" s="75"/>
       <c r="BL23" s="75"/>
       <c r="BM23" s="75"/>
       <c r="BN23" s="75"/>
       <c r="BO23" s="75"/>
-      <c r="BP23" s="76"/>
+      <c r="BP23" s="75"/>
+      <c r="BQ23" s="76"/>
     </row>
-    <row r="24" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="104" t="s">
+      <c r="B24" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="78"/>
+      <c r="C24" s="137">
+        <v>19</v>
+      </c>
+      <c r="D24" s="81"/>
       <c r="E24" s="78"/>
       <c r="F24" s="78"/>
       <c r="G24" s="78"/>
@@ -3573,24 +3591,24 @@
       <c r="J24" s="78"/>
       <c r="K24" s="78"/>
       <c r="L24" s="78"/>
-      <c r="M24" s="79"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="78"/>
+      <c r="M24" s="78"/>
+      <c r="N24" s="79"/>
+      <c r="O24" s="37"/>
       <c r="P24" s="78"/>
       <c r="Q24" s="78"/>
-      <c r="R24" s="8" t="s">
+      <c r="R24" s="78"/>
+      <c r="S24" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="S24" s="107" t="s">
+      <c r="T24" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="T24" s="78"/>
       <c r="U24" s="78"/>
       <c r="V24" s="78"/>
       <c r="W24" s="78"/>
-      <c r="X24" s="80"/>
-      <c r="Y24" s="81"/>
-      <c r="Z24" s="78"/>
+      <c r="X24" s="78"/>
+      <c r="Y24" s="80"/>
+      <c r="Z24" s="81"/>
       <c r="AA24" s="78"/>
       <c r="AB24" s="78"/>
       <c r="AC24" s="78"/>
@@ -3599,54 +3617,57 @@
       <c r="AF24" s="78"/>
       <c r="AG24" s="78"/>
       <c r="AH24" s="78"/>
-      <c r="AI24" s="79"/>
-      <c r="AJ24" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="AI24" s="78"/>
+      <c r="AJ24" s="79"/>
       <c r="AK24" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AL24" s="82"/>
-      <c r="AM24" s="83"/>
+      <c r="AL24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM24" s="82"/>
       <c r="AN24" s="83"/>
-      <c r="AO24" s="84"/>
+      <c r="AO24" s="83"/>
       <c r="AP24" s="84"/>
       <c r="AQ24" s="84"/>
       <c r="AR24" s="84"/>
       <c r="AS24" s="84"/>
-      <c r="AT24" s="85"/>
-      <c r="AU24" s="86"/>
-      <c r="AV24" s="87"/>
-      <c r="AW24" s="84"/>
+      <c r="AT24" s="84"/>
+      <c r="AU24" s="85"/>
+      <c r="AV24" s="86"/>
+      <c r="AW24" s="87"/>
       <c r="AX24" s="84"/>
       <c r="AY24" s="84"/>
-      <c r="AZ24" s="18"/>
+      <c r="AZ24" s="84"/>
       <c r="BA24" s="18"/>
       <c r="BB24" s="18"/>
       <c r="BC24" s="18"/>
       <c r="BD24" s="18"/>
-      <c r="BE24" s="19"/>
-      <c r="BF24" s="100"/>
-      <c r="BG24" s="101"/>
-      <c r="BH24" s="101"/>
-      <c r="BI24" s="101"/>
-      <c r="BJ24" s="101"/>
-      <c r="BK24" s="101"/>
-      <c r="BL24" s="101"/>
-      <c r="BM24" s="101"/>
-      <c r="BN24" s="101"/>
-      <c r="BO24" s="101"/>
-      <c r="BP24" s="102"/>
+      <c r="BE24" s="18"/>
+      <c r="BF24" s="19"/>
+      <c r="BG24" s="99"/>
+      <c r="BH24" s="100"/>
+      <c r="BI24" s="100"/>
+      <c r="BJ24" s="100"/>
+      <c r="BK24" s="100"/>
+      <c r="BL24" s="100"/>
+      <c r="BM24" s="100"/>
+      <c r="BN24" s="100"/>
+      <c r="BO24" s="100"/>
+      <c r="BP24" s="100"/>
+      <c r="BQ24" s="101"/>
     </row>
-    <row r="25" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="108" t="s">
+    <row r="25" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="109" t="s">
+      <c r="B25" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="78"/>
-      <c r="D25" s="78"/>
+      <c r="C25" s="137">
+        <v>6</v>
+      </c>
+      <c r="D25" s="81"/>
       <c r="E25" s="78"/>
       <c r="F25" s="78"/>
       <c r="G25" s="78"/>
@@ -3655,9 +3676,9 @@
       <c r="J25" s="78"/>
       <c r="K25" s="78"/>
       <c r="L25" s="78"/>
-      <c r="M25" s="79"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="37"/>
       <c r="P25" s="78"/>
       <c r="Q25" s="78"/>
       <c r="R25" s="78"/>
@@ -3666,67 +3687,70 @@
       <c r="U25" s="78"/>
       <c r="V25" s="78"/>
       <c r="W25" s="78"/>
-      <c r="X25" s="80"/>
-      <c r="Y25" s="81"/>
-      <c r="Z25" s="78"/>
+      <c r="X25" s="78"/>
+      <c r="Y25" s="80"/>
+      <c r="Z25" s="81"/>
       <c r="AA25" s="78"/>
       <c r="AB25" s="78"/>
       <c r="AC25" s="78"/>
       <c r="AD25" s="78"/>
-      <c r="AE25" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="AE25" s="78"/>
       <c r="AF25" s="8" t="s">
         <v>35</v>
       </c>
       <c r="AG25" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AH25" s="78"/>
-      <c r="AI25" s="79"/>
-      <c r="AJ25" s="37"/>
-      <c r="AK25" s="78"/>
-      <c r="AL25" s="82"/>
-      <c r="AM25" s="83"/>
+      <c r="AH25" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI25" s="78"/>
+      <c r="AJ25" s="79"/>
+      <c r="AK25" s="37"/>
+      <c r="AL25" s="78"/>
+      <c r="AM25" s="82"/>
       <c r="AN25" s="83"/>
-      <c r="AO25" s="84"/>
+      <c r="AO25" s="83"/>
       <c r="AP25" s="84"/>
       <c r="AQ25" s="84"/>
       <c r="AR25" s="84"/>
       <c r="AS25" s="84"/>
-      <c r="AT25" s="85"/>
-      <c r="AU25" s="86"/>
-      <c r="AV25" s="87"/>
-      <c r="AW25" s="84"/>
+      <c r="AT25" s="84"/>
+      <c r="AU25" s="85"/>
+      <c r="AV25" s="86"/>
+      <c r="AW25" s="87"/>
       <c r="AX25" s="84"/>
       <c r="AY25" s="84"/>
-      <c r="AZ25" s="18"/>
+      <c r="AZ25" s="84"/>
       <c r="BA25" s="18"/>
       <c r="BB25" s="18"/>
       <c r="BC25" s="18"/>
       <c r="BD25" s="18"/>
-      <c r="BE25" s="19"/>
-      <c r="BF25" s="100"/>
-      <c r="BG25" s="101"/>
-      <c r="BH25" s="101"/>
-      <c r="BI25" s="101"/>
-      <c r="BJ25" s="101"/>
-      <c r="BK25" s="101"/>
-      <c r="BL25" s="101"/>
-      <c r="BM25" s="101"/>
-      <c r="BN25" s="101"/>
-      <c r="BO25" s="101"/>
-      <c r="BP25" s="102"/>
+      <c r="BE25" s="18"/>
+      <c r="BF25" s="19"/>
+      <c r="BG25" s="99"/>
+      <c r="BH25" s="100"/>
+      <c r="BI25" s="100"/>
+      <c r="BJ25" s="100"/>
+      <c r="BK25" s="100"/>
+      <c r="BL25" s="100"/>
+      <c r="BM25" s="100"/>
+      <c r="BN25" s="100"/>
+      <c r="BO25" s="100"/>
+      <c r="BP25" s="100"/>
+      <c r="BQ25" s="101"/>
     </row>
-    <row r="26" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="104" t="s">
+      <c r="B26" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="78"/>
+      <c r="C26" s="137">
+        <v>26</v>
+      </c>
+      <c r="D26" s="81"/>
       <c r="E26" s="78"/>
       <c r="F26" s="78"/>
       <c r="G26" s="78"/>
@@ -3735,9 +3759,9 @@
       <c r="J26" s="78"/>
       <c r="K26" s="78"/>
       <c r="L26" s="78"/>
-      <c r="M26" s="79"/>
-      <c r="N26" s="37"/>
-      <c r="O26" s="78"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="79"/>
+      <c r="O26" s="37"/>
       <c r="P26" s="78"/>
       <c r="Q26" s="78"/>
       <c r="R26" s="78"/>
@@ -3746,82 +3770,85 @@
       <c r="U26" s="78"/>
       <c r="V26" s="78"/>
       <c r="W26" s="78"/>
-      <c r="X26" s="80"/>
-      <c r="Y26" s="12">
+      <c r="X26" s="78"/>
+      <c r="Y26" s="80"/>
+      <c r="Z26" s="12">
         <v>102</v>
       </c>
-      <c r="Z26" s="8">
+      <c r="AA26" s="8">
         <v>102</v>
       </c>
-      <c r="AA26" s="88" t="s">
+      <c r="AB26" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="AB26" s="78"/>
       <c r="AC26" s="78"/>
       <c r="AD26" s="78"/>
       <c r="AE26" s="78"/>
       <c r="AF26" s="78"/>
       <c r="AG26" s="78"/>
       <c r="AH26" s="78"/>
-      <c r="AI26" s="79"/>
-      <c r="AJ26" s="37"/>
-      <c r="AK26" s="78"/>
-      <c r="AL26" s="82"/>
-      <c r="AM26" s="83"/>
+      <c r="AI26" s="78"/>
+      <c r="AJ26" s="79"/>
+      <c r="AK26" s="37"/>
+      <c r="AL26" s="78"/>
+      <c r="AM26" s="82"/>
       <c r="AN26" s="83"/>
-      <c r="AO26" s="84"/>
+      <c r="AO26" s="83"/>
       <c r="AP26" s="84"/>
       <c r="AQ26" s="84"/>
       <c r="AR26" s="84"/>
       <c r="AS26" s="84"/>
-      <c r="AT26" s="85"/>
-      <c r="AU26" s="86"/>
-      <c r="AV26" s="87"/>
-      <c r="AW26" s="84"/>
+      <c r="AT26" s="84"/>
+      <c r="AU26" s="85"/>
+      <c r="AV26" s="86"/>
+      <c r="AW26" s="87"/>
       <c r="AX26" s="84"/>
       <c r="AY26" s="84"/>
-      <c r="AZ26" s="18"/>
+      <c r="AZ26" s="84"/>
       <c r="BA26" s="18"/>
       <c r="BB26" s="18"/>
       <c r="BC26" s="18"/>
       <c r="BD26" s="18"/>
-      <c r="BE26" s="19"/>
-      <c r="BF26" s="100"/>
-      <c r="BG26" s="101"/>
-      <c r="BH26" s="101"/>
-      <c r="BI26" s="101"/>
-      <c r="BJ26" s="101"/>
-      <c r="BK26" s="101"/>
-      <c r="BL26" s="101"/>
-      <c r="BM26" s="101"/>
-      <c r="BN26" s="101"/>
-      <c r="BO26" s="101"/>
-      <c r="BP26" s="102"/>
+      <c r="BE26" s="18"/>
+      <c r="BF26" s="19"/>
+      <c r="BG26" s="99"/>
+      <c r="BH26" s="100"/>
+      <c r="BI26" s="100"/>
+      <c r="BJ26" s="100"/>
+      <c r="BK26" s="100"/>
+      <c r="BL26" s="100"/>
+      <c r="BM26" s="100"/>
+      <c r="BN26" s="100"/>
+      <c r="BO26" s="100"/>
+      <c r="BP26" s="100"/>
+      <c r="BQ26" s="101"/>
     </row>
-    <row r="27" spans="1:68" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:69" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="104" t="s">
+      <c r="B27" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="37"/>
-      <c r="D27" s="78"/>
+      <c r="C27" s="137">
+        <v>27</v>
+      </c>
+      <c r="D27" s="81"/>
       <c r="E27" s="78"/>
       <c r="F27" s="78"/>
-      <c r="G27" s="8">
-        <v>24</v>
-      </c>
+      <c r="G27" s="78"/>
       <c r="H27" s="8">
         <v>24</v>
       </c>
-      <c r="I27" s="78"/>
+      <c r="I27" s="8">
+        <v>24</v>
+      </c>
       <c r="J27" s="78"/>
       <c r="K27" s="78"/>
       <c r="L27" s="78"/>
-      <c r="M27" s="79"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="78"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="79"/>
+      <c r="O27" s="37"/>
       <c r="P27" s="78"/>
       <c r="Q27" s="78"/>
       <c r="R27" s="78"/>
@@ -3830,9 +3857,9 @@
       <c r="U27" s="78"/>
       <c r="V27" s="78"/>
       <c r="W27" s="78"/>
-      <c r="X27" s="80"/>
-      <c r="Y27" s="81"/>
-      <c r="Z27" s="78"/>
+      <c r="X27" s="78"/>
+      <c r="Y27" s="80"/>
+      <c r="Z27" s="81"/>
       <c r="AA27" s="78"/>
       <c r="AB27" s="78"/>
       <c r="AC27" s="78"/>
@@ -3841,33 +3868,33 @@
       <c r="AF27" s="78"/>
       <c r="AG27" s="78"/>
       <c r="AH27" s="78"/>
-      <c r="AI27" s="79"/>
-      <c r="AJ27" s="37"/>
-      <c r="AK27" s="78"/>
-      <c r="AL27" s="82"/>
-      <c r="AM27" s="83"/>
+      <c r="AI27" s="78"/>
+      <c r="AJ27" s="79"/>
+      <c r="AK27" s="37"/>
+      <c r="AL27" s="78"/>
+      <c r="AM27" s="82"/>
       <c r="AN27" s="83"/>
-      <c r="AO27" s="84"/>
+      <c r="AO27" s="83"/>
       <c r="AP27" s="84"/>
       <c r="AQ27" s="84"/>
       <c r="AR27" s="84"/>
       <c r="AS27" s="84"/>
-      <c r="AT27" s="85"/>
-      <c r="AU27" s="86"/>
-      <c r="AV27" s="87"/>
-      <c r="AW27" s="88" t="s">
+      <c r="AT27" s="84"/>
+      <c r="AU27" s="85"/>
+      <c r="AV27" s="86"/>
+      <c r="AW27" s="87"/>
+      <c r="AX27" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="AX27" s="84"/>
       <c r="AY27" s="84"/>
-      <c r="AZ27" s="18"/>
+      <c r="AZ27" s="84"/>
       <c r="BA27" s="18"/>
       <c r="BB27" s="18"/>
       <c r="BC27" s="18"/>
       <c r="BD27" s="18"/>
-      <c r="BE27" s="19"/>
-      <c r="BF27" s="42"/>
-      <c r="BG27" s="43"/>
+      <c r="BE27" s="18"/>
+      <c r="BF27" s="19"/>
+      <c r="BG27" s="42"/>
       <c r="BH27" s="43"/>
       <c r="BI27" s="43"/>
       <c r="BJ27" s="43"/>
@@ -3876,17 +3903,20 @@
       <c r="BM27" s="43"/>
       <c r="BN27" s="43"/>
       <c r="BO27" s="43"/>
-      <c r="BP27" s="44"/>
+      <c r="BP27" s="43"/>
+      <c r="BQ27" s="44"/>
     </row>
-    <row r="28" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="104" t="s">
+      <c r="B28" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="78"/>
+      <c r="C28" s="137">
+        <v>8</v>
+      </c>
+      <c r="D28" s="81"/>
       <c r="E28" s="78"/>
       <c r="F28" s="78"/>
       <c r="G28" s="78"/>
@@ -3895,59 +3925,59 @@
       <c r="J28" s="78"/>
       <c r="K28" s="78"/>
       <c r="L28" s="78"/>
-      <c r="M28" s="79"/>
-      <c r="N28" s="37"/>
-      <c r="O28" s="48"/>
-      <c r="P28" s="8">
-        <v>24</v>
-      </c>
+      <c r="M28" s="78"/>
+      <c r="N28" s="79"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="48"/>
       <c r="Q28" s="8">
         <v>24</v>
       </c>
       <c r="R28" s="8">
         <v>24</v>
       </c>
-      <c r="S28" s="48"/>
+      <c r="S28" s="8">
+        <v>24</v>
+      </c>
       <c r="T28" s="48"/>
       <c r="U28" s="48"/>
-      <c r="V28" s="78"/>
+      <c r="V28" s="48"/>
       <c r="W28" s="78"/>
-      <c r="X28" s="80"/>
-      <c r="Y28" s="110"/>
-      <c r="Z28" s="110"/>
-      <c r="AA28" s="110"/>
-      <c r="AB28" s="110"/>
-      <c r="AC28" s="111"/>
-      <c r="AD28" s="111"/>
+      <c r="X28" s="78"/>
+      <c r="Y28" s="80"/>
+      <c r="Z28" s="109"/>
+      <c r="AA28" s="109"/>
+      <c r="AB28" s="109"/>
+      <c r="AC28" s="109"/>
+      <c r="AD28" s="110"/>
       <c r="AE28" s="110"/>
-      <c r="AF28" s="110"/>
-      <c r="AG28" s="110"/>
-      <c r="AH28" s="110"/>
-      <c r="AI28" s="110"/>
-      <c r="AJ28" s="110"/>
-      <c r="AK28" s="110"/>
-      <c r="AL28" s="110"/>
-      <c r="AM28" s="112"/>
-      <c r="AN28" s="83"/>
-      <c r="AO28" s="110"/>
-      <c r="AP28" s="110"/>
-      <c r="AQ28" s="110"/>
-      <c r="AR28" s="110"/>
-      <c r="AS28" s="110"/>
-      <c r="AT28" s="110"/>
-      <c r="AU28" s="110"/>
-      <c r="AV28" s="110"/>
-      <c r="AW28" s="110"/>
-      <c r="AX28" s="113"/>
-      <c r="AY28" s="113"/>
-      <c r="AZ28" s="114"/>
-      <c r="BA28" s="114"/>
-      <c r="BB28" s="114"/>
-      <c r="BC28" s="114"/>
-      <c r="BD28" s="114"/>
-      <c r="BE28" s="114"/>
-      <c r="BF28" s="115"/>
-      <c r="BG28" s="75"/>
+      <c r="AF28" s="109"/>
+      <c r="AG28" s="109"/>
+      <c r="AH28" s="109"/>
+      <c r="AI28" s="109"/>
+      <c r="AJ28" s="109"/>
+      <c r="AK28" s="109"/>
+      <c r="AL28" s="109"/>
+      <c r="AM28" s="109"/>
+      <c r="AN28" s="111"/>
+      <c r="AO28" s="83"/>
+      <c r="AP28" s="109"/>
+      <c r="AQ28" s="109"/>
+      <c r="AR28" s="109"/>
+      <c r="AS28" s="109"/>
+      <c r="AT28" s="109"/>
+      <c r="AU28" s="109"/>
+      <c r="AV28" s="109"/>
+      <c r="AW28" s="109"/>
+      <c r="AX28" s="109"/>
+      <c r="AY28" s="112"/>
+      <c r="AZ28" s="112"/>
+      <c r="BA28" s="113"/>
+      <c r="BB28" s="113"/>
+      <c r="BC28" s="113"/>
+      <c r="BD28" s="113"/>
+      <c r="BE28" s="113"/>
+      <c r="BF28" s="113"/>
+      <c r="BG28" s="114"/>
       <c r="BH28" s="75"/>
       <c r="BI28" s="75"/>
       <c r="BJ28" s="75"/>
@@ -3956,17 +3986,20 @@
       <c r="BM28" s="75"/>
       <c r="BN28" s="75"/>
       <c r="BO28" s="75"/>
-      <c r="BP28" s="76"/>
+      <c r="BP28" s="75"/>
+      <c r="BQ28" s="76"/>
     </row>
-    <row r="29" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="104" t="s">
+      <c r="B29" s="103" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="78"/>
+      <c r="C29" s="137">
+        <v>8</v>
+      </c>
+      <c r="D29" s="81"/>
       <c r="E29" s="78"/>
       <c r="F29" s="78"/>
       <c r="G29" s="78"/>
@@ -3975,57 +4008,57 @@
       <c r="J29" s="78"/>
       <c r="K29" s="78"/>
       <c r="L29" s="78"/>
-      <c r="M29" s="79"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="48"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="37"/>
       <c r="P29" s="48"/>
       <c r="Q29" s="48"/>
       <c r="R29" s="48"/>
       <c r="S29" s="48"/>
-      <c r="T29" s="116">
+      <c r="T29" s="48"/>
+      <c r="U29" s="115">
         <v>23</v>
       </c>
-      <c r="U29" s="116">
+      <c r="V29" s="115">
         <v>23</v>
       </c>
-      <c r="V29" s="78"/>
       <c r="W29" s="78"/>
-      <c r="X29" s="80"/>
-      <c r="Y29" s="117"/>
-      <c r="Z29" s="118"/>
-      <c r="AA29" s="118"/>
-      <c r="AB29" s="118"/>
-      <c r="AC29" s="119"/>
-      <c r="AD29" s="119"/>
+      <c r="X29" s="78"/>
+      <c r="Y29" s="80"/>
+      <c r="Z29" s="116"/>
+      <c r="AA29" s="117"/>
+      <c r="AB29" s="117"/>
+      <c r="AC29" s="117"/>
+      <c r="AD29" s="118"/>
       <c r="AE29" s="118"/>
-      <c r="AF29" s="118"/>
-      <c r="AG29" s="118"/>
-      <c r="AH29" s="118"/>
-      <c r="AI29" s="120"/>
-      <c r="AJ29" s="117"/>
-      <c r="AK29" s="118"/>
-      <c r="AL29" s="118"/>
-      <c r="AM29" s="121"/>
-      <c r="AN29" s="122"/>
-      <c r="AO29" s="118"/>
-      <c r="AP29" s="118"/>
-      <c r="AQ29" s="118"/>
-      <c r="AR29" s="118"/>
-      <c r="AS29" s="118"/>
-      <c r="AT29" s="120"/>
-      <c r="AU29" s="117"/>
-      <c r="AV29" s="118"/>
-      <c r="AW29" s="118"/>
-      <c r="AX29" s="105"/>
-      <c r="AY29" s="105"/>
-      <c r="AZ29" s="91"/>
+      <c r="AF29" s="117"/>
+      <c r="AG29" s="117"/>
+      <c r="AH29" s="117"/>
+      <c r="AI29" s="117"/>
+      <c r="AJ29" s="119"/>
+      <c r="AK29" s="116"/>
+      <c r="AL29" s="117"/>
+      <c r="AM29" s="117"/>
+      <c r="AN29" s="120"/>
+      <c r="AO29" s="121"/>
+      <c r="AP29" s="117"/>
+      <c r="AQ29" s="117"/>
+      <c r="AR29" s="117"/>
+      <c r="AS29" s="117"/>
+      <c r="AT29" s="117"/>
+      <c r="AU29" s="119"/>
+      <c r="AV29" s="116"/>
+      <c r="AW29" s="117"/>
+      <c r="AX29" s="117"/>
+      <c r="AY29" s="104"/>
+      <c r="AZ29" s="104"/>
       <c r="BA29" s="91"/>
       <c r="BB29" s="91"/>
       <c r="BC29" s="91"/>
       <c r="BD29" s="91"/>
-      <c r="BE29" s="93"/>
-      <c r="BF29" s="42"/>
-      <c r="BG29" s="43"/>
+      <c r="BE29" s="91"/>
+      <c r="BF29" s="93"/>
+      <c r="BG29" s="42"/>
       <c r="BH29" s="43"/>
       <c r="BI29" s="43"/>
       <c r="BJ29" s="43"/>
@@ -4034,17 +4067,20 @@
       <c r="BM29" s="43"/>
       <c r="BN29" s="43"/>
       <c r="BO29" s="43"/>
-      <c r="BP29" s="44"/>
+      <c r="BP29" s="43"/>
+      <c r="BQ29" s="44"/>
     </row>
-    <row r="30" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="104" t="s">
+      <c r="B30" s="103" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="78"/>
+      <c r="C30" s="137">
+        <v>8</v>
+      </c>
+      <c r="D30" s="81"/>
       <c r="E30" s="78"/>
       <c r="F30" s="78"/>
       <c r="G30" s="78"/>
@@ -4053,78 +4089,81 @@
       <c r="J30" s="78"/>
       <c r="K30" s="78"/>
       <c r="L30" s="78"/>
-      <c r="M30" s="79"/>
-      <c r="N30" s="37"/>
-      <c r="O30" s="78"/>
+      <c r="M30" s="78"/>
+      <c r="N30" s="79"/>
+      <c r="O30" s="37"/>
       <c r="P30" s="78"/>
       <c r="Q30" s="78"/>
       <c r="R30" s="78"/>
       <c r="S30" s="78"/>
-      <c r="T30" s="123">
-        <f>T29</f>
-        <v>23</v>
-      </c>
-      <c r="U30" s="123">
+      <c r="T30" s="78"/>
+      <c r="U30" s="122">
         <f>U29</f>
         <v>23</v>
       </c>
-      <c r="V30" s="78"/>
+      <c r="V30" s="122">
+        <f>V29</f>
+        <v>23</v>
+      </c>
       <c r="W30" s="78"/>
-      <c r="X30" s="80"/>
-      <c r="Y30" s="124"/>
-      <c r="Z30" s="110"/>
-      <c r="AA30" s="110"/>
-      <c r="AB30" s="110"/>
-      <c r="AC30" s="110"/>
-      <c r="AD30" s="110"/>
-      <c r="AE30" s="110"/>
-      <c r="AF30" s="110"/>
-      <c r="AG30" s="110"/>
-      <c r="AH30" s="110"/>
-      <c r="AI30" s="125"/>
+      <c r="X30" s="78"/>
+      <c r="Y30" s="80"/>
+      <c r="Z30" s="123"/>
+      <c r="AA30" s="109"/>
+      <c r="AB30" s="109"/>
+      <c r="AC30" s="109"/>
+      <c r="AD30" s="109"/>
+      <c r="AE30" s="109"/>
+      <c r="AF30" s="109"/>
+      <c r="AG30" s="109"/>
+      <c r="AH30" s="109"/>
+      <c r="AI30" s="109"/>
       <c r="AJ30" s="124"/>
-      <c r="AK30" s="110"/>
-      <c r="AL30" s="110"/>
-      <c r="AM30" s="112"/>
-      <c r="AN30" s="83"/>
-      <c r="AO30" s="110"/>
-      <c r="AP30" s="110"/>
-      <c r="AQ30" s="110"/>
-      <c r="AR30" s="110"/>
-      <c r="AS30" s="110"/>
-      <c r="AT30" s="125"/>
+      <c r="AK30" s="123"/>
+      <c r="AL30" s="109"/>
+      <c r="AM30" s="109"/>
+      <c r="AN30" s="111"/>
+      <c r="AO30" s="83"/>
+      <c r="AP30" s="109"/>
+      <c r="AQ30" s="109"/>
+      <c r="AR30" s="109"/>
+      <c r="AS30" s="109"/>
+      <c r="AT30" s="109"/>
       <c r="AU30" s="124"/>
-      <c r="AV30" s="110"/>
-      <c r="AW30" s="110"/>
-      <c r="AX30" s="113"/>
-      <c r="AY30" s="113"/>
-      <c r="AZ30" s="114"/>
-      <c r="BA30" s="114"/>
-      <c r="BB30" s="114"/>
-      <c r="BC30" s="114"/>
-      <c r="BD30" s="114"/>
-      <c r="BE30" s="126"/>
-      <c r="BF30" s="127"/>
-      <c r="BG30" s="114"/>
-      <c r="BH30" s="114"/>
+      <c r="AV30" s="123"/>
+      <c r="AW30" s="109"/>
+      <c r="AX30" s="109"/>
+      <c r="AY30" s="112"/>
+      <c r="AZ30" s="112"/>
+      <c r="BA30" s="113"/>
+      <c r="BB30" s="113"/>
+      <c r="BC30" s="113"/>
+      <c r="BD30" s="113"/>
+      <c r="BE30" s="113"/>
+      <c r="BF30" s="125"/>
+      <c r="BG30" s="126"/>
+      <c r="BH30" s="113"/>
       <c r="BI30" s="113"/>
-      <c r="BJ30" s="113"/>
-      <c r="BK30" s="114"/>
-      <c r="BL30" s="43"/>
+      <c r="BJ30" s="112"/>
+      <c r="BK30" s="112"/>
+      <c r="BL30" s="113"/>
       <c r="BM30" s="43"/>
       <c r="BN30" s="43"/>
       <c r="BO30" s="43"/>
-      <c r="BP30" s="44"/>
+      <c r="BP30" s="43"/>
+      <c r="BQ30" s="44"/>
     </row>
-    <row r="31" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="104" t="s">
+      <c r="B31" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="37"/>
-      <c r="D31" s="78"/>
+      <c r="C31" s="137">
+        <v>9</v>
+      </c>
+      <c r="D31" s="81"/>
       <c r="E31" s="78"/>
       <c r="F31" s="78"/>
       <c r="G31" s="78"/>
@@ -4133,24 +4172,24 @@
       <c r="J31" s="78"/>
       <c r="K31" s="78"/>
       <c r="L31" s="78"/>
-      <c r="M31" s="79"/>
-      <c r="N31" s="128" t="s">
+      <c r="M31" s="78"/>
+      <c r="N31" s="79"/>
+      <c r="O31" s="127" t="s">
         <v>66</v>
       </c>
-      <c r="O31" s="116" t="s">
+      <c r="P31" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="P31" s="48"/>
-      <c r="Q31" s="78"/>
+      <c r="Q31" s="48"/>
       <c r="R31" s="78"/>
       <c r="S31" s="78"/>
       <c r="T31" s="78"/>
       <c r="U31" s="78"/>
       <c r="V31" s="78"/>
       <c r="W31" s="78"/>
-      <c r="X31" s="80"/>
-      <c r="Y31" s="81"/>
-      <c r="Z31" s="78"/>
+      <c r="X31" s="78"/>
+      <c r="Y31" s="80"/>
+      <c r="Z31" s="81"/>
       <c r="AA31" s="78"/>
       <c r="AB31" s="78"/>
       <c r="AC31" s="78"/>
@@ -4158,51 +4197,54 @@
       <c r="AE31" s="78"/>
       <c r="AF31" s="78"/>
       <c r="AG31" s="78"/>
-      <c r="AH31" s="35"/>
-      <c r="AI31" s="36"/>
-      <c r="AJ31" s="127"/>
-      <c r="AK31" s="114"/>
-      <c r="AL31" s="114"/>
-      <c r="AM31" s="92"/>
+      <c r="AH31" s="78"/>
+      <c r="AI31" s="35"/>
+      <c r="AJ31" s="36"/>
+      <c r="AK31" s="126"/>
+      <c r="AL31" s="113"/>
+      <c r="AM31" s="113"/>
       <c r="AN31" s="92"/>
-      <c r="AO31" s="114"/>
-      <c r="AP31" s="114"/>
-      <c r="AQ31" s="129"/>
-      <c r="AR31" s="25"/>
-      <c r="AS31" s="114"/>
-      <c r="AT31" s="114"/>
-      <c r="AU31" s="127"/>
-      <c r="AV31" s="114"/>
-      <c r="AW31" s="114"/>
+      <c r="AO31" s="92"/>
+      <c r="AP31" s="113"/>
+      <c r="AQ31" s="113"/>
+      <c r="AR31" s="128"/>
+      <c r="AS31" s="25"/>
+      <c r="AT31" s="113"/>
+      <c r="AU31" s="113"/>
+      <c r="AV31" s="126"/>
+      <c r="AW31" s="113"/>
       <c r="AX31" s="113"/>
-      <c r="AY31" s="113"/>
-      <c r="AZ31" s="113"/>
-      <c r="BA31" s="114"/>
-      <c r="BB31" s="114"/>
-      <c r="BC31" s="114"/>
-      <c r="BD31" s="114"/>
-      <c r="BE31" s="126"/>
-      <c r="BF31" s="127"/>
-      <c r="BG31" s="114"/>
-      <c r="BH31" s="114"/>
-      <c r="BI31" s="114"/>
-      <c r="BJ31" s="114"/>
-      <c r="BK31" s="114"/>
-      <c r="BL31" s="114"/>
-      <c r="BM31" s="114"/>
-      <c r="BN31" s="114"/>
-      <c r="BO31" s="114"/>
-      <c r="BP31" s="126"/>
+      <c r="AY31" s="112"/>
+      <c r="AZ31" s="112"/>
+      <c r="BA31" s="112"/>
+      <c r="BB31" s="113"/>
+      <c r="BC31" s="113"/>
+      <c r="BD31" s="113"/>
+      <c r="BE31" s="113"/>
+      <c r="BF31" s="125"/>
+      <c r="BG31" s="126"/>
+      <c r="BH31" s="113"/>
+      <c r="BI31" s="113"/>
+      <c r="BJ31" s="113"/>
+      <c r="BK31" s="113"/>
+      <c r="BL31" s="113"/>
+      <c r="BM31" s="113"/>
+      <c r="BN31" s="113"/>
+      <c r="BO31" s="113"/>
+      <c r="BP31" s="113"/>
+      <c r="BQ31" s="125"/>
     </row>
-    <row r="32" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="104" t="s">
+      <c r="B32" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="78"/>
+      <c r="C32" s="137">
+        <v>9</v>
+      </c>
+      <c r="D32" s="81"/>
       <c r="E32" s="78"/>
       <c r="F32" s="78"/>
       <c r="G32" s="78"/>
@@ -4211,16 +4253,16 @@
       <c r="J32" s="78"/>
       <c r="K32" s="78"/>
       <c r="L32" s="78"/>
-      <c r="M32" s="79"/>
-      <c r="N32" s="123" t="str">
-        <f>N31</f>
-        <v>X</v>
-      </c>
-      <c r="O32" s="123" t="str">
+      <c r="M32" s="78"/>
+      <c r="N32" s="79"/>
+      <c r="O32" s="122" t="str">
         <f>O31</f>
         <v>X</v>
       </c>
-      <c r="P32" s="78"/>
+      <c r="P32" s="122" t="str">
+        <f>P31</f>
+        <v>X</v>
+      </c>
       <c r="Q32" s="78"/>
       <c r="R32" s="78"/>
       <c r="S32" s="78"/>
@@ -4228,9 +4270,9 @@
       <c r="U32" s="78"/>
       <c r="V32" s="78"/>
       <c r="W32" s="78"/>
-      <c r="X32" s="80"/>
-      <c r="Y32" s="81"/>
-      <c r="Z32" s="78"/>
+      <c r="X32" s="78"/>
+      <c r="Y32" s="80"/>
+      <c r="Z32" s="81"/>
       <c r="AA32" s="78"/>
       <c r="AB32" s="78"/>
       <c r="AC32" s="78"/>
@@ -4238,68 +4280,71 @@
       <c r="AE32" s="78"/>
       <c r="AF32" s="78"/>
       <c r="AG32" s="78"/>
-      <c r="AH32" s="35"/>
-      <c r="AI32" s="36"/>
-      <c r="AJ32" s="127"/>
-      <c r="AK32" s="114"/>
-      <c r="AL32" s="114"/>
-      <c r="AM32" s="92"/>
+      <c r="AH32" s="78"/>
+      <c r="AI32" s="35"/>
+      <c r="AJ32" s="36"/>
+      <c r="AK32" s="126"/>
+      <c r="AL32" s="113"/>
+      <c r="AM32" s="113"/>
       <c r="AN32" s="92"/>
-      <c r="AO32" s="114"/>
-      <c r="AP32" s="114"/>
-      <c r="AQ32" s="129"/>
-      <c r="AR32" s="25"/>
-      <c r="AS32" s="114"/>
-      <c r="AT32" s="114"/>
-      <c r="AU32" s="127"/>
-      <c r="AV32" s="114"/>
-      <c r="AW32" s="114"/>
+      <c r="AO32" s="92"/>
+      <c r="AP32" s="113"/>
+      <c r="AQ32" s="113"/>
+      <c r="AR32" s="128"/>
+      <c r="AS32" s="25"/>
+      <c r="AT32" s="113"/>
+      <c r="AU32" s="113"/>
+      <c r="AV32" s="126"/>
+      <c r="AW32" s="113"/>
       <c r="AX32" s="113"/>
-      <c r="AY32" s="113"/>
-      <c r="AZ32" s="113"/>
-      <c r="BA32" s="114"/>
-      <c r="BB32" s="114"/>
-      <c r="BC32" s="114"/>
-      <c r="BD32" s="114"/>
-      <c r="BE32" s="126"/>
-      <c r="BF32" s="127"/>
-      <c r="BG32" s="114"/>
-      <c r="BH32" s="114"/>
-      <c r="BI32" s="114"/>
-      <c r="BJ32" s="114"/>
-      <c r="BK32" s="114"/>
-      <c r="BL32" s="114"/>
-      <c r="BM32" s="114"/>
-      <c r="BN32" s="114"/>
-      <c r="BO32" s="114"/>
-      <c r="BP32" s="126"/>
+      <c r="AY32" s="112"/>
+      <c r="AZ32" s="112"/>
+      <c r="BA32" s="112"/>
+      <c r="BB32" s="113"/>
+      <c r="BC32" s="113"/>
+      <c r="BD32" s="113"/>
+      <c r="BE32" s="113"/>
+      <c r="BF32" s="125"/>
+      <c r="BG32" s="126"/>
+      <c r="BH32" s="113"/>
+      <c r="BI32" s="113"/>
+      <c r="BJ32" s="113"/>
+      <c r="BK32" s="113"/>
+      <c r="BL32" s="113"/>
+      <c r="BM32" s="113"/>
+      <c r="BN32" s="113"/>
+      <c r="BO32" s="113"/>
+      <c r="BP32" s="113"/>
+      <c r="BQ32" s="125"/>
     </row>
-    <row r="33" spans="1:68" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:69" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="104" t="s">
+      <c r="B33" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="10">
-        <v>25</v>
-      </c>
-      <c r="D33" s="8">
+      <c r="C33" s="137">
+        <v>5</v>
+      </c>
+      <c r="D33" s="12">
         <v>25</v>
       </c>
       <c r="E33" s="8">
         <v>25</v>
       </c>
-      <c r="F33" s="48"/>
+      <c r="F33" s="8">
+        <v>25</v>
+      </c>
       <c r="G33" s="48"/>
-      <c r="H33" s="78"/>
+      <c r="H33" s="48"/>
       <c r="I33" s="78"/>
       <c r="J33" s="78"/>
       <c r="K33" s="78"/>
       <c r="L33" s="78"/>
-      <c r="M33" s="79"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="78"/>
+      <c r="M33" s="78"/>
+      <c r="N33" s="79"/>
+      <c r="O33" s="37"/>
       <c r="P33" s="78"/>
       <c r="Q33" s="78"/>
       <c r="R33" s="78"/>
@@ -4308,9 +4353,9 @@
       <c r="U33" s="78"/>
       <c r="V33" s="78"/>
       <c r="W33" s="78"/>
-      <c r="X33" s="80"/>
-      <c r="Y33" s="81"/>
-      <c r="Z33" s="78"/>
+      <c r="X33" s="78"/>
+      <c r="Y33" s="80"/>
+      <c r="Z33" s="81"/>
       <c r="AA33" s="78"/>
       <c r="AB33" s="78"/>
       <c r="AC33" s="78"/>
@@ -4318,92 +4363,97 @@
       <c r="AE33" s="78"/>
       <c r="AF33" s="78"/>
       <c r="AG33" s="78"/>
-      <c r="AH33" s="35"/>
-      <c r="AI33" s="36"/>
-      <c r="AJ33" s="127"/>
-      <c r="AK33" s="114"/>
-      <c r="AL33" s="114"/>
-      <c r="AM33" s="92"/>
+      <c r="AH33" s="78"/>
+      <c r="AI33" s="35"/>
+      <c r="AJ33" s="36"/>
+      <c r="AK33" s="126"/>
+      <c r="AL33" s="113"/>
+      <c r="AM33" s="113"/>
       <c r="AN33" s="92"/>
-      <c r="AO33" s="114"/>
-      <c r="AP33" s="114"/>
-      <c r="AQ33" s="129"/>
-      <c r="AR33" s="114"/>
-      <c r="AS33" s="114"/>
-      <c r="AT33" s="114"/>
-      <c r="AU33" s="127"/>
-      <c r="AV33" s="114"/>
-      <c r="AW33" s="114"/>
+      <c r="AO33" s="92"/>
+      <c r="AP33" s="113"/>
+      <c r="AQ33" s="113"/>
+      <c r="AR33" s="128"/>
+      <c r="AS33" s="113"/>
+      <c r="AT33" s="113"/>
+      <c r="AU33" s="113"/>
+      <c r="AV33" s="126"/>
+      <c r="AW33" s="113"/>
       <c r="AX33" s="113"/>
-      <c r="AY33" s="113"/>
-      <c r="AZ33" s="113"/>
-      <c r="BA33" s="114"/>
-      <c r="BB33" s="114"/>
-      <c r="BC33" s="114"/>
-      <c r="BD33" s="114"/>
-      <c r="BE33" s="126"/>
-      <c r="BF33" s="127"/>
-      <c r="BG33" s="114"/>
-      <c r="BH33" s="114"/>
-      <c r="BI33" s="114"/>
-      <c r="BJ33" s="114"/>
-      <c r="BK33" s="114"/>
-      <c r="BL33" s="114"/>
-      <c r="BM33" s="114"/>
-      <c r="BN33" s="114"/>
-      <c r="BO33" s="114"/>
-      <c r="BP33" s="126"/>
+      <c r="AY33" s="112"/>
+      <c r="AZ33" s="112"/>
+      <c r="BA33" s="112"/>
+      <c r="BB33" s="113"/>
+      <c r="BC33" s="113"/>
+      <c r="BD33" s="113"/>
+      <c r="BE33" s="113"/>
+      <c r="BF33" s="125"/>
+      <c r="BG33" s="126"/>
+      <c r="BH33" s="113"/>
+      <c r="BI33" s="113"/>
+      <c r="BJ33" s="113"/>
+      <c r="BK33" s="113"/>
+      <c r="BL33" s="113"/>
+      <c r="BM33" s="113"/>
+      <c r="BN33" s="113"/>
+      <c r="BO33" s="113"/>
+      <c r="BP33" s="113"/>
+      <c r="BQ33" s="125"/>
+    </row>
+    <row r="34" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="C34" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="N1:X1"/>
-    <mergeCell ref="Y1:AI1"/>
-    <mergeCell ref="AJ1:AT1"/>
-    <mergeCell ref="AU1:BE1"/>
-    <mergeCell ref="BF1:BP1"/>
+    <mergeCell ref="BG1:BQ1"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="O1:Y1"/>
+    <mergeCell ref="Z1:AJ1"/>
+    <mergeCell ref="AK1:AU1"/>
+    <mergeCell ref="AV1:BF1"/>
   </mergeCells>
-  <conditionalFormatting sqref="X1">
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",X1)))</formula>
+  <conditionalFormatting sqref="Y1">
+    <cfRule type="containsText" dxfId="7" priority="18" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",Y1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X8 X12:X15 X18:X30">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",X8)))</formula>
+  <conditionalFormatting sqref="Y8 Y12:Y15 Y18:Y30">
+    <cfRule type="containsText" dxfId="6" priority="17" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",Y8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X31">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",X31)))</formula>
+  <conditionalFormatting sqref="Y31">
+    <cfRule type="containsText" dxfId="5" priority="16" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",Y31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X7">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",X2)))</formula>
+  <conditionalFormatting sqref="Y2:Y7">
+    <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",Y2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X32:X33">
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",X32)))</formula>
+  <conditionalFormatting sqref="Y32:Y33">
+    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",Y32)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X10:X11">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",X10)))</formula>
+  <conditionalFormatting sqref="Y10:Y11">
+    <cfRule type="containsText" dxfId="2" priority="11" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",Y10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X9">
-    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",X9)))</formula>
+  <conditionalFormatting sqref="Y9">
+    <cfRule type="containsText" dxfId="1" priority="13" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",Y9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X16:X17">
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",X16)))</formula>
+  <conditionalFormatting sqref="Y16:Y17">
+    <cfRule type="containsText" dxfId="0" priority="12" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",Y16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>